<commit_message>
Updated columns for sections.
</commit_message>
<xml_diff>
--- a/inst/extdata/QA_Template_Coded_Analysis.xlsx
+++ b/inst/extdata/QA_Template_Coded_Analysis.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzadra41/Documents/R Projects/integral-private/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B71DAFF7-906C-B544-B32D-B2E8C6334644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF59A3D3-D50D-0D40-AA21-6DDFE4AE2FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31980" yWindow="11160" windowWidth="38140" windowHeight="24120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31960" yWindow="11120" windowWidth="38140" windowHeight="24120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA Instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="Code_Review" sheetId="3" r:id="rId2"/>
+    <sheet name="Code_Review_Template" sheetId="3" state="hidden" r:id="rId2"/>
     <sheet name="QA Tags" sheetId="4" r:id="rId3"/>
     <sheet name="Resources" sheetId="6" r:id="rId4"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="87">
   <si>
     <t>Privileged and Confidential</t>
   </si>
@@ -244,10 +244,6 @@
     <t>Section</t>
   </si>
   <si>
-    <t>Lines or Reference Location
-(subject to change)</t>
-  </si>
-  <si>
     <t>Review Instructions</t>
   </si>
   <si>
@@ -283,19 +279,7 @@
 (Initials, rationale, or confirmation that issue was corrected in the code)</t>
   </si>
   <si>
-    <t>Insert section header or general category</t>
-  </si>
-  <si>
-    <t>Insert line numbers</t>
-  </si>
-  <si>
     <t>#tag</t>
-  </si>
-  <si>
-    <t>Add more lines per section as needed</t>
-  </si>
-  <si>
-    <t>Add more sections as needed</t>
   </si>
   <si>
     <r>
@@ -481,6 +465,18 @@
   </si>
   <si>
     <t>QA ID</t>
+  </si>
+  <si>
+    <t>Line Number (Approximate)</t>
+  </si>
+  <si>
+    <t>Subsection</t>
+  </si>
+  <si>
+    <t>Level 3</t>
+  </si>
+  <si>
+    <t>Level 4</t>
   </si>
 </sst>
 </file>
@@ -766,7 +762,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -1034,6 +1030,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1045,7 +1061,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="154">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1372,6 +1388,12 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1405,12 +1427,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="20" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1420,15 +1436,9 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1441,9 +1451,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1466,6 +1473,12 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="23" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1539,7 +1552,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" checked="Checked" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1849,13 +1862,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -1916,16 +1929,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>11289</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1983,13 +1996,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -2050,13 +2063,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -2117,13 +2130,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -2184,13 +2197,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
@@ -2251,13 +2264,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
@@ -2318,16 +2331,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2385,16 +2398,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2452,13 +2465,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -2519,13 +2532,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -2586,13 +2599,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>203200</xdr:rowOff>
@@ -2653,13 +2666,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -2720,13 +2733,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -2787,13 +2800,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -2854,13 +2867,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -2921,13 +2934,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -2988,13 +3001,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
@@ -3055,13 +3068,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
@@ -3122,13 +3135,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
@@ -3189,16 +3202,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3256,16 +3269,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3323,16 +3336,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3390,13 +3403,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -3457,13 +3470,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -3524,13 +3537,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -3591,13 +3604,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>203200</xdr:rowOff>
@@ -3658,13 +3671,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>203200</xdr:rowOff>
@@ -3725,13 +3738,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -3792,13 +3805,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -3859,13 +3872,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -3926,13 +3939,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -3993,13 +4006,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4060,13 +4073,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4127,13 +4140,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4194,13 +4207,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4261,13 +4274,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4328,13 +4341,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4395,16 +4408,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4462,16 +4475,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4529,16 +4542,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4596,16 +4609,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4663,16 +4676,16 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>9</xdr:row>
-          <xdr:rowOff>25400</xdr:rowOff>
+          <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4730,13 +4743,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -4797,13 +4810,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4864,13 +4877,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -4931,13 +4944,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -4998,13 +5011,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -5065,13 +5078,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5132,13 +5145,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5199,13 +5212,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -5266,13 +5279,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -5333,13 +5346,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5400,13 +5413,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5467,13 +5480,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5534,13 +5547,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -5601,13 +5614,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -5668,13 +5681,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
@@ -5735,13 +5748,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5802,13 +5815,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2844800</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>609601</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
@@ -5869,13 +5882,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>2832100</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>5</xdr:col>
+          <xdr:col>8</xdr:col>
           <xdr:colOff>114301</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>63500</xdr:rowOff>
@@ -6329,22 +6342,22 @@
       <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="124"/>
-      <c r="C5" s="124"/>
-      <c r="D5" s="124"/>
-      <c r="E5" s="124"/>
+      <c r="B5" s="126"/>
+      <c r="C5" s="126"/>
+      <c r="D5" s="126"/>
+      <c r="E5" s="126"/>
       <c r="F5" s="38"/>
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
       <c r="J5" s="39"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="122" t="s">
+      <c r="B6" s="124" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="122"/>
-      <c r="D6" s="122"/>
-      <c r="E6" s="122"/>
+      <c r="C6" s="124"/>
+      <c r="D6" s="124"/>
+      <c r="E6" s="124"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.15">
       <c r="D7" s="43"/>
@@ -6354,62 +6367,62 @@
       <c r="A8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="123"/>
-      <c r="C8" s="123"/>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
+      <c r="B8" s="125"/>
+      <c r="C8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
+      <c r="B9" s="125"/>
+      <c r="C9" s="125"/>
+      <c r="D9" s="125"/>
+      <c r="E9" s="125"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="123"/>
-      <c r="C10" s="123"/>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
+      <c r="B10" s="125"/>
+      <c r="C10" s="125"/>
+      <c r="D10" s="125"/>
+      <c r="E10" s="125"/>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.15">
       <c r="A11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="123"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
+      <c r="B11" s="125"/>
+      <c r="C11" s="125"/>
+      <c r="D11" s="125"/>
+      <c r="E11" s="125"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="123"/>
-      <c r="C12" s="123"/>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
+      <c r="B12" s="125"/>
+      <c r="C12" s="125"/>
+      <c r="D12" s="125"/>
+      <c r="E12" s="125"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A13" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="123"/>
-      <c r="C13" s="123"/>
-      <c r="D13" s="123"/>
-      <c r="E13" s="123"/>
+      <c r="B13" s="125"/>
+      <c r="C13" s="125"/>
+      <c r="D13" s="125"/>
+      <c r="E13" s="125"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="47"/>
-      <c r="B14" s="123"/>
-      <c r="C14" s="123"/>
-      <c r="D14" s="123"/>
-      <c r="E14" s="123"/>
+      <c r="B14" s="125"/>
+      <c r="C14" s="125"/>
+      <c r="D14" s="125"/>
+      <c r="E14" s="125"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="48"/>
@@ -6438,9 +6451,9 @@
       <c r="B17" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="129"/>
-      <c r="D17" s="129"/>
-      <c r="E17" s="130"/>
+      <c r="C17" s="131"/>
+      <c r="D17" s="131"/>
+      <c r="E17" s="132"/>
       <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -6450,9 +6463,9 @@
       <c r="B18" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="131"/>
-      <c r="D18" s="131"/>
-      <c r="E18" s="132"/>
+      <c r="C18" s="133"/>
+      <c r="D18" s="133"/>
+      <c r="E18" s="134"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
@@ -6461,9 +6474,9 @@
       <c r="B19" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="131"/>
-      <c r="D19" s="131"/>
-      <c r="E19" s="132"/>
+      <c r="C19" s="133"/>
+      <c r="D19" s="133"/>
+      <c r="E19" s="134"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
@@ -6472,16 +6485,16 @@
       <c r="B20" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="125"/>
-      <c r="D20" s="125"/>
-      <c r="E20" s="126"/>
+      <c r="C20" s="127"/>
+      <c r="D20" s="127"/>
+      <c r="E20" s="128"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="28"/>
       <c r="B21" s="90"/>
-      <c r="C21" s="125"/>
-      <c r="D21" s="125"/>
-      <c r="E21" s="126"/>
+      <c r="C21" s="127"/>
+      <c r="D21" s="127"/>
+      <c r="E21" s="128"/>
     </row>
     <row r="22" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A22" s="28" t="s">
@@ -6490,9 +6503,9 @@
       <c r="B22" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="127"/>
-      <c r="D22" s="127"/>
-      <c r="E22" s="128"/>
+      <c r="C22" s="129"/>
+      <c r="D22" s="129"/>
+      <c r="E22" s="130"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="28"/>
@@ -6721,707 +6734,722 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:BM120"/>
+  <dimension ref="A1:BP120"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" style="15" customWidth="1"/>
-    <col min="2" max="3" width="20.6640625" style="15" customWidth="1"/>
-    <col min="4" max="4" width="42.5" style="15" customWidth="1"/>
-    <col min="5" max="5" width="3" style="15" customWidth="1"/>
-    <col min="6" max="6" width="44" style="15" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" style="15" customWidth="1"/>
-    <col min="8" max="8" width="17.5" style="15" customWidth="1"/>
-    <col min="9" max="9" width="13.33203125" style="15" customWidth="1"/>
-    <col min="10" max="10" width="27.6640625" style="15" customWidth="1"/>
-    <col min="11" max="11" width="2.5" style="21" customWidth="1"/>
-    <col min="12" max="12" width="19.5" style="15" customWidth="1"/>
-    <col min="13" max="13" width="18.83203125" style="15" customWidth="1"/>
-    <col min="14" max="14" width="14" style="15" customWidth="1"/>
-    <col min="15" max="15" width="15.33203125" style="15" customWidth="1"/>
-    <col min="16" max="16" width="8" style="15" customWidth="1"/>
-    <col min="17" max="17" width="28.1640625" style="15" customWidth="1"/>
-    <col min="18" max="260" width="9.1640625" style="15"/>
-    <col min="261" max="261" width="15.5" style="15" customWidth="1"/>
-    <col min="262" max="262" width="27.83203125" style="15" customWidth="1"/>
-    <col min="263" max="263" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="33.1640625" style="15" customWidth="1"/>
-    <col min="265" max="265" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="9.1640625" style="15"/>
-    <col min="267" max="267" width="17.83203125" style="15" customWidth="1"/>
-    <col min="268" max="516" width="9.1640625" style="15"/>
-    <col min="517" max="517" width="15.5" style="15" customWidth="1"/>
-    <col min="518" max="518" width="27.83203125" style="15" customWidth="1"/>
-    <col min="519" max="519" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="520" max="520" width="33.1640625" style="15" customWidth="1"/>
-    <col min="521" max="521" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="522" max="522" width="9.1640625" style="15"/>
-    <col min="523" max="523" width="17.83203125" style="15" customWidth="1"/>
-    <col min="524" max="772" width="9.1640625" style="15"/>
-    <col min="773" max="773" width="15.5" style="15" customWidth="1"/>
-    <col min="774" max="774" width="27.83203125" style="15" customWidth="1"/>
-    <col min="775" max="775" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="776" max="776" width="33.1640625" style="15" customWidth="1"/>
-    <col min="777" max="777" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="778" max="778" width="9.1640625" style="15"/>
-    <col min="779" max="779" width="17.83203125" style="15" customWidth="1"/>
-    <col min="780" max="1028" width="9.1640625" style="15"/>
-    <col min="1029" max="1029" width="15.5" style="15" customWidth="1"/>
-    <col min="1030" max="1030" width="27.83203125" style="15" customWidth="1"/>
-    <col min="1031" max="1031" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="1032" max="1032" width="33.1640625" style="15" customWidth="1"/>
-    <col min="1033" max="1033" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="1034" max="1034" width="9.1640625" style="15"/>
-    <col min="1035" max="1035" width="17.83203125" style="15" customWidth="1"/>
-    <col min="1036" max="1284" width="9.1640625" style="15"/>
-    <col min="1285" max="1285" width="15.5" style="15" customWidth="1"/>
-    <col min="1286" max="1286" width="27.83203125" style="15" customWidth="1"/>
-    <col min="1287" max="1287" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="1288" max="1288" width="33.1640625" style="15" customWidth="1"/>
-    <col min="1289" max="1289" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="1290" max="1290" width="9.1640625" style="15"/>
-    <col min="1291" max="1291" width="17.83203125" style="15" customWidth="1"/>
-    <col min="1292" max="1540" width="9.1640625" style="15"/>
-    <col min="1541" max="1541" width="15.5" style="15" customWidth="1"/>
-    <col min="1542" max="1542" width="27.83203125" style="15" customWidth="1"/>
-    <col min="1543" max="1543" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="1544" max="1544" width="33.1640625" style="15" customWidth="1"/>
-    <col min="1545" max="1545" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="1546" max="1546" width="9.1640625" style="15"/>
-    <col min="1547" max="1547" width="17.83203125" style="15" customWidth="1"/>
-    <col min="1548" max="1796" width="9.1640625" style="15"/>
-    <col min="1797" max="1797" width="15.5" style="15" customWidth="1"/>
-    <col min="1798" max="1798" width="27.83203125" style="15" customWidth="1"/>
-    <col min="1799" max="1799" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="1800" max="1800" width="33.1640625" style="15" customWidth="1"/>
-    <col min="1801" max="1801" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="1802" max="1802" width="9.1640625" style="15"/>
-    <col min="1803" max="1803" width="17.83203125" style="15" customWidth="1"/>
-    <col min="1804" max="2052" width="9.1640625" style="15"/>
-    <col min="2053" max="2053" width="15.5" style="15" customWidth="1"/>
-    <col min="2054" max="2054" width="27.83203125" style="15" customWidth="1"/>
-    <col min="2055" max="2055" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="2056" max="2056" width="33.1640625" style="15" customWidth="1"/>
-    <col min="2057" max="2057" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="2058" max="2058" width="9.1640625" style="15"/>
-    <col min="2059" max="2059" width="17.83203125" style="15" customWidth="1"/>
-    <col min="2060" max="2308" width="9.1640625" style="15"/>
-    <col min="2309" max="2309" width="15.5" style="15" customWidth="1"/>
-    <col min="2310" max="2310" width="27.83203125" style="15" customWidth="1"/>
-    <col min="2311" max="2311" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="2312" max="2312" width="33.1640625" style="15" customWidth="1"/>
-    <col min="2313" max="2313" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="2314" max="2314" width="9.1640625" style="15"/>
-    <col min="2315" max="2315" width="17.83203125" style="15" customWidth="1"/>
-    <col min="2316" max="2564" width="9.1640625" style="15"/>
-    <col min="2565" max="2565" width="15.5" style="15" customWidth="1"/>
-    <col min="2566" max="2566" width="27.83203125" style="15" customWidth="1"/>
-    <col min="2567" max="2567" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="2568" max="2568" width="33.1640625" style="15" customWidth="1"/>
-    <col min="2569" max="2569" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="2570" max="2570" width="9.1640625" style="15"/>
-    <col min="2571" max="2571" width="17.83203125" style="15" customWidth="1"/>
-    <col min="2572" max="2820" width="9.1640625" style="15"/>
-    <col min="2821" max="2821" width="15.5" style="15" customWidth="1"/>
-    <col min="2822" max="2822" width="27.83203125" style="15" customWidth="1"/>
-    <col min="2823" max="2823" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="2824" max="2824" width="33.1640625" style="15" customWidth="1"/>
-    <col min="2825" max="2825" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="2826" max="2826" width="9.1640625" style="15"/>
-    <col min="2827" max="2827" width="17.83203125" style="15" customWidth="1"/>
-    <col min="2828" max="3076" width="9.1640625" style="15"/>
-    <col min="3077" max="3077" width="15.5" style="15" customWidth="1"/>
-    <col min="3078" max="3078" width="27.83203125" style="15" customWidth="1"/>
-    <col min="3079" max="3079" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="3080" max="3080" width="33.1640625" style="15" customWidth="1"/>
-    <col min="3081" max="3081" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="3082" max="3082" width="9.1640625" style="15"/>
-    <col min="3083" max="3083" width="17.83203125" style="15" customWidth="1"/>
-    <col min="3084" max="3332" width="9.1640625" style="15"/>
-    <col min="3333" max="3333" width="15.5" style="15" customWidth="1"/>
-    <col min="3334" max="3334" width="27.83203125" style="15" customWidth="1"/>
-    <col min="3335" max="3335" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="3336" max="3336" width="33.1640625" style="15" customWidth="1"/>
-    <col min="3337" max="3337" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="3338" max="3338" width="9.1640625" style="15"/>
-    <col min="3339" max="3339" width="17.83203125" style="15" customWidth="1"/>
-    <col min="3340" max="3588" width="9.1640625" style="15"/>
-    <col min="3589" max="3589" width="15.5" style="15" customWidth="1"/>
-    <col min="3590" max="3590" width="27.83203125" style="15" customWidth="1"/>
-    <col min="3591" max="3591" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="3592" max="3592" width="33.1640625" style="15" customWidth="1"/>
-    <col min="3593" max="3593" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="3594" max="3594" width="9.1640625" style="15"/>
-    <col min="3595" max="3595" width="17.83203125" style="15" customWidth="1"/>
-    <col min="3596" max="3844" width="9.1640625" style="15"/>
-    <col min="3845" max="3845" width="15.5" style="15" customWidth="1"/>
-    <col min="3846" max="3846" width="27.83203125" style="15" customWidth="1"/>
-    <col min="3847" max="3847" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="3848" max="3848" width="33.1640625" style="15" customWidth="1"/>
-    <col min="3849" max="3849" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="3850" max="3850" width="9.1640625" style="15"/>
-    <col min="3851" max="3851" width="17.83203125" style="15" customWidth="1"/>
-    <col min="3852" max="4100" width="9.1640625" style="15"/>
-    <col min="4101" max="4101" width="15.5" style="15" customWidth="1"/>
-    <col min="4102" max="4102" width="27.83203125" style="15" customWidth="1"/>
-    <col min="4103" max="4103" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="4104" max="4104" width="33.1640625" style="15" customWidth="1"/>
-    <col min="4105" max="4105" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="4106" max="4106" width="9.1640625" style="15"/>
-    <col min="4107" max="4107" width="17.83203125" style="15" customWidth="1"/>
-    <col min="4108" max="4356" width="9.1640625" style="15"/>
-    <col min="4357" max="4357" width="15.5" style="15" customWidth="1"/>
-    <col min="4358" max="4358" width="27.83203125" style="15" customWidth="1"/>
-    <col min="4359" max="4359" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="4360" max="4360" width="33.1640625" style="15" customWidth="1"/>
-    <col min="4361" max="4361" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="4362" max="4362" width="9.1640625" style="15"/>
-    <col min="4363" max="4363" width="17.83203125" style="15" customWidth="1"/>
-    <col min="4364" max="4612" width="9.1640625" style="15"/>
-    <col min="4613" max="4613" width="15.5" style="15" customWidth="1"/>
-    <col min="4614" max="4614" width="27.83203125" style="15" customWidth="1"/>
-    <col min="4615" max="4615" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="4616" max="4616" width="33.1640625" style="15" customWidth="1"/>
-    <col min="4617" max="4617" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="4618" max="4618" width="9.1640625" style="15"/>
-    <col min="4619" max="4619" width="17.83203125" style="15" customWidth="1"/>
-    <col min="4620" max="4868" width="9.1640625" style="15"/>
-    <col min="4869" max="4869" width="15.5" style="15" customWidth="1"/>
-    <col min="4870" max="4870" width="27.83203125" style="15" customWidth="1"/>
-    <col min="4871" max="4871" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="4872" max="4872" width="33.1640625" style="15" customWidth="1"/>
-    <col min="4873" max="4873" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="4874" max="4874" width="9.1640625" style="15"/>
-    <col min="4875" max="4875" width="17.83203125" style="15" customWidth="1"/>
-    <col min="4876" max="5124" width="9.1640625" style="15"/>
-    <col min="5125" max="5125" width="15.5" style="15" customWidth="1"/>
-    <col min="5126" max="5126" width="27.83203125" style="15" customWidth="1"/>
-    <col min="5127" max="5127" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="5128" max="5128" width="33.1640625" style="15" customWidth="1"/>
-    <col min="5129" max="5129" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="5130" max="5130" width="9.1640625" style="15"/>
-    <col min="5131" max="5131" width="17.83203125" style="15" customWidth="1"/>
-    <col min="5132" max="5380" width="9.1640625" style="15"/>
-    <col min="5381" max="5381" width="15.5" style="15" customWidth="1"/>
-    <col min="5382" max="5382" width="27.83203125" style="15" customWidth="1"/>
-    <col min="5383" max="5383" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="5384" max="5384" width="33.1640625" style="15" customWidth="1"/>
-    <col min="5385" max="5385" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="5386" max="5386" width="9.1640625" style="15"/>
-    <col min="5387" max="5387" width="17.83203125" style="15" customWidth="1"/>
-    <col min="5388" max="5636" width="9.1640625" style="15"/>
-    <col min="5637" max="5637" width="15.5" style="15" customWidth="1"/>
-    <col min="5638" max="5638" width="27.83203125" style="15" customWidth="1"/>
-    <col min="5639" max="5639" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="5640" max="5640" width="33.1640625" style="15" customWidth="1"/>
-    <col min="5641" max="5641" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="5642" max="5642" width="9.1640625" style="15"/>
-    <col min="5643" max="5643" width="17.83203125" style="15" customWidth="1"/>
-    <col min="5644" max="5892" width="9.1640625" style="15"/>
-    <col min="5893" max="5893" width="15.5" style="15" customWidth="1"/>
-    <col min="5894" max="5894" width="27.83203125" style="15" customWidth="1"/>
-    <col min="5895" max="5895" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="5896" max="5896" width="33.1640625" style="15" customWidth="1"/>
-    <col min="5897" max="5897" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="5898" max="5898" width="9.1640625" style="15"/>
-    <col min="5899" max="5899" width="17.83203125" style="15" customWidth="1"/>
-    <col min="5900" max="6148" width="9.1640625" style="15"/>
-    <col min="6149" max="6149" width="15.5" style="15" customWidth="1"/>
-    <col min="6150" max="6150" width="27.83203125" style="15" customWidth="1"/>
-    <col min="6151" max="6151" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="6152" max="6152" width="33.1640625" style="15" customWidth="1"/>
-    <col min="6153" max="6153" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="6154" max="6154" width="9.1640625" style="15"/>
-    <col min="6155" max="6155" width="17.83203125" style="15" customWidth="1"/>
-    <col min="6156" max="6404" width="9.1640625" style="15"/>
-    <col min="6405" max="6405" width="15.5" style="15" customWidth="1"/>
-    <col min="6406" max="6406" width="27.83203125" style="15" customWidth="1"/>
-    <col min="6407" max="6407" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="6408" max="6408" width="33.1640625" style="15" customWidth="1"/>
-    <col min="6409" max="6409" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="6410" max="6410" width="9.1640625" style="15"/>
-    <col min="6411" max="6411" width="17.83203125" style="15" customWidth="1"/>
-    <col min="6412" max="6660" width="9.1640625" style="15"/>
-    <col min="6661" max="6661" width="15.5" style="15" customWidth="1"/>
-    <col min="6662" max="6662" width="27.83203125" style="15" customWidth="1"/>
-    <col min="6663" max="6663" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="6664" max="6664" width="33.1640625" style="15" customWidth="1"/>
-    <col min="6665" max="6665" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="6666" max="6666" width="9.1640625" style="15"/>
-    <col min="6667" max="6667" width="17.83203125" style="15" customWidth="1"/>
-    <col min="6668" max="6916" width="9.1640625" style="15"/>
-    <col min="6917" max="6917" width="15.5" style="15" customWidth="1"/>
-    <col min="6918" max="6918" width="27.83203125" style="15" customWidth="1"/>
-    <col min="6919" max="6919" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="6920" max="6920" width="33.1640625" style="15" customWidth="1"/>
-    <col min="6921" max="6921" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="6922" max="6922" width="9.1640625" style="15"/>
-    <col min="6923" max="6923" width="17.83203125" style="15" customWidth="1"/>
-    <col min="6924" max="7172" width="9.1640625" style="15"/>
-    <col min="7173" max="7173" width="15.5" style="15" customWidth="1"/>
-    <col min="7174" max="7174" width="27.83203125" style="15" customWidth="1"/>
-    <col min="7175" max="7175" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="7176" max="7176" width="33.1640625" style="15" customWidth="1"/>
-    <col min="7177" max="7177" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="7178" max="7178" width="9.1640625" style="15"/>
-    <col min="7179" max="7179" width="17.83203125" style="15" customWidth="1"/>
-    <col min="7180" max="7428" width="9.1640625" style="15"/>
-    <col min="7429" max="7429" width="15.5" style="15" customWidth="1"/>
-    <col min="7430" max="7430" width="27.83203125" style="15" customWidth="1"/>
-    <col min="7431" max="7431" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="7432" max="7432" width="33.1640625" style="15" customWidth="1"/>
-    <col min="7433" max="7433" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="7434" max="7434" width="9.1640625" style="15"/>
-    <col min="7435" max="7435" width="17.83203125" style="15" customWidth="1"/>
-    <col min="7436" max="7684" width="9.1640625" style="15"/>
-    <col min="7685" max="7685" width="15.5" style="15" customWidth="1"/>
-    <col min="7686" max="7686" width="27.83203125" style="15" customWidth="1"/>
-    <col min="7687" max="7687" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="7688" max="7688" width="33.1640625" style="15" customWidth="1"/>
-    <col min="7689" max="7689" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="7690" max="7690" width="9.1640625" style="15"/>
-    <col min="7691" max="7691" width="17.83203125" style="15" customWidth="1"/>
-    <col min="7692" max="7940" width="9.1640625" style="15"/>
-    <col min="7941" max="7941" width="15.5" style="15" customWidth="1"/>
-    <col min="7942" max="7942" width="27.83203125" style="15" customWidth="1"/>
-    <col min="7943" max="7943" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="7944" max="7944" width="33.1640625" style="15" customWidth="1"/>
-    <col min="7945" max="7945" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="7946" max="7946" width="9.1640625" style="15"/>
-    <col min="7947" max="7947" width="17.83203125" style="15" customWidth="1"/>
-    <col min="7948" max="8196" width="9.1640625" style="15"/>
-    <col min="8197" max="8197" width="15.5" style="15" customWidth="1"/>
-    <col min="8198" max="8198" width="27.83203125" style="15" customWidth="1"/>
-    <col min="8199" max="8199" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="8200" max="8200" width="33.1640625" style="15" customWidth="1"/>
-    <col min="8201" max="8201" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="8202" max="8202" width="9.1640625" style="15"/>
-    <col min="8203" max="8203" width="17.83203125" style="15" customWidth="1"/>
-    <col min="8204" max="8452" width="9.1640625" style="15"/>
-    <col min="8453" max="8453" width="15.5" style="15" customWidth="1"/>
-    <col min="8454" max="8454" width="27.83203125" style="15" customWidth="1"/>
-    <col min="8455" max="8455" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="8456" max="8456" width="33.1640625" style="15" customWidth="1"/>
-    <col min="8457" max="8457" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="8458" max="8458" width="9.1640625" style="15"/>
-    <col min="8459" max="8459" width="17.83203125" style="15" customWidth="1"/>
-    <col min="8460" max="8708" width="9.1640625" style="15"/>
-    <col min="8709" max="8709" width="15.5" style="15" customWidth="1"/>
-    <col min="8710" max="8710" width="27.83203125" style="15" customWidth="1"/>
-    <col min="8711" max="8711" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="8712" max="8712" width="33.1640625" style="15" customWidth="1"/>
-    <col min="8713" max="8713" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="8714" max="8714" width="9.1640625" style="15"/>
-    <col min="8715" max="8715" width="17.83203125" style="15" customWidth="1"/>
-    <col min="8716" max="8964" width="9.1640625" style="15"/>
-    <col min="8965" max="8965" width="15.5" style="15" customWidth="1"/>
-    <col min="8966" max="8966" width="27.83203125" style="15" customWidth="1"/>
-    <col min="8967" max="8967" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="8968" max="8968" width="33.1640625" style="15" customWidth="1"/>
-    <col min="8969" max="8969" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="8970" max="8970" width="9.1640625" style="15"/>
-    <col min="8971" max="8971" width="17.83203125" style="15" customWidth="1"/>
-    <col min="8972" max="9220" width="9.1640625" style="15"/>
-    <col min="9221" max="9221" width="15.5" style="15" customWidth="1"/>
-    <col min="9222" max="9222" width="27.83203125" style="15" customWidth="1"/>
-    <col min="9223" max="9223" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="9224" max="9224" width="33.1640625" style="15" customWidth="1"/>
-    <col min="9225" max="9225" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="9226" max="9226" width="9.1640625" style="15"/>
-    <col min="9227" max="9227" width="17.83203125" style="15" customWidth="1"/>
-    <col min="9228" max="9476" width="9.1640625" style="15"/>
-    <col min="9477" max="9477" width="15.5" style="15" customWidth="1"/>
-    <col min="9478" max="9478" width="27.83203125" style="15" customWidth="1"/>
-    <col min="9479" max="9479" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="9480" max="9480" width="33.1640625" style="15" customWidth="1"/>
-    <col min="9481" max="9481" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="9482" max="9482" width="9.1640625" style="15"/>
-    <col min="9483" max="9483" width="17.83203125" style="15" customWidth="1"/>
-    <col min="9484" max="9732" width="9.1640625" style="15"/>
-    <col min="9733" max="9733" width="15.5" style="15" customWidth="1"/>
-    <col min="9734" max="9734" width="27.83203125" style="15" customWidth="1"/>
-    <col min="9735" max="9735" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="9736" max="9736" width="33.1640625" style="15" customWidth="1"/>
-    <col min="9737" max="9737" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="9738" max="9738" width="9.1640625" style="15"/>
-    <col min="9739" max="9739" width="17.83203125" style="15" customWidth="1"/>
-    <col min="9740" max="9988" width="9.1640625" style="15"/>
-    <col min="9989" max="9989" width="15.5" style="15" customWidth="1"/>
-    <col min="9990" max="9990" width="27.83203125" style="15" customWidth="1"/>
-    <col min="9991" max="9991" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="9992" max="9992" width="33.1640625" style="15" customWidth="1"/>
-    <col min="9993" max="9993" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="9994" max="9994" width="9.1640625" style="15"/>
-    <col min="9995" max="9995" width="17.83203125" style="15" customWidth="1"/>
-    <col min="9996" max="10244" width="9.1640625" style="15"/>
-    <col min="10245" max="10245" width="15.5" style="15" customWidth="1"/>
-    <col min="10246" max="10246" width="27.83203125" style="15" customWidth="1"/>
-    <col min="10247" max="10247" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="10248" max="10248" width="33.1640625" style="15" customWidth="1"/>
-    <col min="10249" max="10249" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="10250" max="10250" width="9.1640625" style="15"/>
-    <col min="10251" max="10251" width="17.83203125" style="15" customWidth="1"/>
-    <col min="10252" max="10500" width="9.1640625" style="15"/>
-    <col min="10501" max="10501" width="15.5" style="15" customWidth="1"/>
-    <col min="10502" max="10502" width="27.83203125" style="15" customWidth="1"/>
-    <col min="10503" max="10503" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="10504" max="10504" width="33.1640625" style="15" customWidth="1"/>
-    <col min="10505" max="10505" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="10506" max="10506" width="9.1640625" style="15"/>
-    <col min="10507" max="10507" width="17.83203125" style="15" customWidth="1"/>
-    <col min="10508" max="10756" width="9.1640625" style="15"/>
-    <col min="10757" max="10757" width="15.5" style="15" customWidth="1"/>
-    <col min="10758" max="10758" width="27.83203125" style="15" customWidth="1"/>
-    <col min="10759" max="10759" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="10760" max="10760" width="33.1640625" style="15" customWidth="1"/>
-    <col min="10761" max="10761" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="10762" max="10762" width="9.1640625" style="15"/>
-    <col min="10763" max="10763" width="17.83203125" style="15" customWidth="1"/>
-    <col min="10764" max="11012" width="9.1640625" style="15"/>
-    <col min="11013" max="11013" width="15.5" style="15" customWidth="1"/>
-    <col min="11014" max="11014" width="27.83203125" style="15" customWidth="1"/>
-    <col min="11015" max="11015" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="11016" max="11016" width="33.1640625" style="15" customWidth="1"/>
-    <col min="11017" max="11017" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="11018" max="11018" width="9.1640625" style="15"/>
-    <col min="11019" max="11019" width="17.83203125" style="15" customWidth="1"/>
-    <col min="11020" max="11268" width="9.1640625" style="15"/>
-    <col min="11269" max="11269" width="15.5" style="15" customWidth="1"/>
-    <col min="11270" max="11270" width="27.83203125" style="15" customWidth="1"/>
-    <col min="11271" max="11271" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="11272" max="11272" width="33.1640625" style="15" customWidth="1"/>
-    <col min="11273" max="11273" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="11274" max="11274" width="9.1640625" style="15"/>
-    <col min="11275" max="11275" width="17.83203125" style="15" customWidth="1"/>
-    <col min="11276" max="11524" width="9.1640625" style="15"/>
-    <col min="11525" max="11525" width="15.5" style="15" customWidth="1"/>
-    <col min="11526" max="11526" width="27.83203125" style="15" customWidth="1"/>
-    <col min="11527" max="11527" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="11528" max="11528" width="33.1640625" style="15" customWidth="1"/>
-    <col min="11529" max="11529" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="11530" max="11530" width="9.1640625" style="15"/>
-    <col min="11531" max="11531" width="17.83203125" style="15" customWidth="1"/>
-    <col min="11532" max="11780" width="9.1640625" style="15"/>
-    <col min="11781" max="11781" width="15.5" style="15" customWidth="1"/>
-    <col min="11782" max="11782" width="27.83203125" style="15" customWidth="1"/>
-    <col min="11783" max="11783" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="11784" max="11784" width="33.1640625" style="15" customWidth="1"/>
-    <col min="11785" max="11785" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="11786" max="11786" width="9.1640625" style="15"/>
-    <col min="11787" max="11787" width="17.83203125" style="15" customWidth="1"/>
-    <col min="11788" max="12036" width="9.1640625" style="15"/>
-    <col min="12037" max="12037" width="15.5" style="15" customWidth="1"/>
-    <col min="12038" max="12038" width="27.83203125" style="15" customWidth="1"/>
-    <col min="12039" max="12039" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="12040" max="12040" width="33.1640625" style="15" customWidth="1"/>
-    <col min="12041" max="12041" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="12042" max="12042" width="9.1640625" style="15"/>
-    <col min="12043" max="12043" width="17.83203125" style="15" customWidth="1"/>
-    <col min="12044" max="12292" width="9.1640625" style="15"/>
-    <col min="12293" max="12293" width="15.5" style="15" customWidth="1"/>
-    <col min="12294" max="12294" width="27.83203125" style="15" customWidth="1"/>
-    <col min="12295" max="12295" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="12296" max="12296" width="33.1640625" style="15" customWidth="1"/>
-    <col min="12297" max="12297" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="12298" max="12298" width="9.1640625" style="15"/>
-    <col min="12299" max="12299" width="17.83203125" style="15" customWidth="1"/>
-    <col min="12300" max="12548" width="9.1640625" style="15"/>
-    <col min="12549" max="12549" width="15.5" style="15" customWidth="1"/>
-    <col min="12550" max="12550" width="27.83203125" style="15" customWidth="1"/>
-    <col min="12551" max="12551" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="12552" max="12552" width="33.1640625" style="15" customWidth="1"/>
-    <col min="12553" max="12553" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="12554" max="12554" width="9.1640625" style="15"/>
-    <col min="12555" max="12555" width="17.83203125" style="15" customWidth="1"/>
-    <col min="12556" max="12804" width="9.1640625" style="15"/>
-    <col min="12805" max="12805" width="15.5" style="15" customWidth="1"/>
-    <col min="12806" max="12806" width="27.83203125" style="15" customWidth="1"/>
-    <col min="12807" max="12807" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="12808" max="12808" width="33.1640625" style="15" customWidth="1"/>
-    <col min="12809" max="12809" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="12810" max="12810" width="9.1640625" style="15"/>
-    <col min="12811" max="12811" width="17.83203125" style="15" customWidth="1"/>
-    <col min="12812" max="13060" width="9.1640625" style="15"/>
-    <col min="13061" max="13061" width="15.5" style="15" customWidth="1"/>
-    <col min="13062" max="13062" width="27.83203125" style="15" customWidth="1"/>
-    <col min="13063" max="13063" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="13064" max="13064" width="33.1640625" style="15" customWidth="1"/>
-    <col min="13065" max="13065" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="13066" max="13066" width="9.1640625" style="15"/>
-    <col min="13067" max="13067" width="17.83203125" style="15" customWidth="1"/>
-    <col min="13068" max="13316" width="9.1640625" style="15"/>
-    <col min="13317" max="13317" width="15.5" style="15" customWidth="1"/>
-    <col min="13318" max="13318" width="27.83203125" style="15" customWidth="1"/>
-    <col min="13319" max="13319" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="13320" max="13320" width="33.1640625" style="15" customWidth="1"/>
-    <col min="13321" max="13321" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="13322" max="13322" width="9.1640625" style="15"/>
-    <col min="13323" max="13323" width="17.83203125" style="15" customWidth="1"/>
-    <col min="13324" max="13572" width="9.1640625" style="15"/>
-    <col min="13573" max="13573" width="15.5" style="15" customWidth="1"/>
-    <col min="13574" max="13574" width="27.83203125" style="15" customWidth="1"/>
-    <col min="13575" max="13575" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="13576" max="13576" width="33.1640625" style="15" customWidth="1"/>
-    <col min="13577" max="13577" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="13578" max="13578" width="9.1640625" style="15"/>
-    <col min="13579" max="13579" width="17.83203125" style="15" customWidth="1"/>
-    <col min="13580" max="13828" width="9.1640625" style="15"/>
-    <col min="13829" max="13829" width="15.5" style="15" customWidth="1"/>
-    <col min="13830" max="13830" width="27.83203125" style="15" customWidth="1"/>
-    <col min="13831" max="13831" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="13832" max="13832" width="33.1640625" style="15" customWidth="1"/>
-    <col min="13833" max="13833" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="13834" max="13834" width="9.1640625" style="15"/>
-    <col min="13835" max="13835" width="17.83203125" style="15" customWidth="1"/>
-    <col min="13836" max="14084" width="9.1640625" style="15"/>
-    <col min="14085" max="14085" width="15.5" style="15" customWidth="1"/>
-    <col min="14086" max="14086" width="27.83203125" style="15" customWidth="1"/>
-    <col min="14087" max="14087" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="14088" max="14088" width="33.1640625" style="15" customWidth="1"/>
-    <col min="14089" max="14089" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="14090" max="14090" width="9.1640625" style="15"/>
-    <col min="14091" max="14091" width="17.83203125" style="15" customWidth="1"/>
-    <col min="14092" max="14340" width="9.1640625" style="15"/>
-    <col min="14341" max="14341" width="15.5" style="15" customWidth="1"/>
-    <col min="14342" max="14342" width="27.83203125" style="15" customWidth="1"/>
-    <col min="14343" max="14343" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="14344" max="14344" width="33.1640625" style="15" customWidth="1"/>
-    <col min="14345" max="14345" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="14346" max="14346" width="9.1640625" style="15"/>
-    <col min="14347" max="14347" width="17.83203125" style="15" customWidth="1"/>
-    <col min="14348" max="14596" width="9.1640625" style="15"/>
-    <col min="14597" max="14597" width="15.5" style="15" customWidth="1"/>
-    <col min="14598" max="14598" width="27.83203125" style="15" customWidth="1"/>
-    <col min="14599" max="14599" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="14600" max="14600" width="33.1640625" style="15" customWidth="1"/>
-    <col min="14601" max="14601" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="14602" max="14602" width="9.1640625" style="15"/>
-    <col min="14603" max="14603" width="17.83203125" style="15" customWidth="1"/>
-    <col min="14604" max="14852" width="9.1640625" style="15"/>
-    <col min="14853" max="14853" width="15.5" style="15" customWidth="1"/>
-    <col min="14854" max="14854" width="27.83203125" style="15" customWidth="1"/>
-    <col min="14855" max="14855" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="14856" max="14856" width="33.1640625" style="15" customWidth="1"/>
-    <col min="14857" max="14857" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="14858" max="14858" width="9.1640625" style="15"/>
-    <col min="14859" max="14859" width="17.83203125" style="15" customWidth="1"/>
-    <col min="14860" max="15108" width="9.1640625" style="15"/>
-    <col min="15109" max="15109" width="15.5" style="15" customWidth="1"/>
-    <col min="15110" max="15110" width="27.83203125" style="15" customWidth="1"/>
-    <col min="15111" max="15111" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="15112" max="15112" width="33.1640625" style="15" customWidth="1"/>
-    <col min="15113" max="15113" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="15114" max="15114" width="9.1640625" style="15"/>
-    <col min="15115" max="15115" width="17.83203125" style="15" customWidth="1"/>
-    <col min="15116" max="15364" width="9.1640625" style="15"/>
-    <col min="15365" max="15365" width="15.5" style="15" customWidth="1"/>
-    <col min="15366" max="15366" width="27.83203125" style="15" customWidth="1"/>
-    <col min="15367" max="15367" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="15368" max="15368" width="33.1640625" style="15" customWidth="1"/>
-    <col min="15369" max="15369" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="15370" max="15370" width="9.1640625" style="15"/>
-    <col min="15371" max="15371" width="17.83203125" style="15" customWidth="1"/>
-    <col min="15372" max="15620" width="9.1640625" style="15"/>
-    <col min="15621" max="15621" width="15.5" style="15" customWidth="1"/>
-    <col min="15622" max="15622" width="27.83203125" style="15" customWidth="1"/>
-    <col min="15623" max="15623" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="15624" max="15624" width="33.1640625" style="15" customWidth="1"/>
-    <col min="15625" max="15625" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="15626" max="15626" width="9.1640625" style="15"/>
-    <col min="15627" max="15627" width="17.83203125" style="15" customWidth="1"/>
-    <col min="15628" max="15876" width="9.1640625" style="15"/>
-    <col min="15877" max="15877" width="15.5" style="15" customWidth="1"/>
-    <col min="15878" max="15878" width="27.83203125" style="15" customWidth="1"/>
-    <col min="15879" max="15879" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="15880" max="15880" width="33.1640625" style="15" customWidth="1"/>
-    <col min="15881" max="15881" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="15882" max="15882" width="9.1640625" style="15"/>
-    <col min="15883" max="15883" width="17.83203125" style="15" customWidth="1"/>
-    <col min="15884" max="16132" width="9.1640625" style="15"/>
-    <col min="16133" max="16133" width="15.5" style="15" customWidth="1"/>
-    <col min="16134" max="16134" width="27.83203125" style="15" customWidth="1"/>
-    <col min="16135" max="16135" width="68" style="15" bestFit="1" customWidth="1"/>
-    <col min="16136" max="16136" width="33.1640625" style="15" customWidth="1"/>
-    <col min="16137" max="16137" width="8" style="15" bestFit="1" customWidth="1"/>
-    <col min="16138" max="16138" width="9.1640625" style="15"/>
-    <col min="16139" max="16139" width="17.83203125" style="15" customWidth="1"/>
-    <col min="16140" max="16384" width="9.1640625" style="15"/>
+    <col min="1" max="4" width="18.33203125" style="15" customWidth="1"/>
+    <col min="5" max="6" width="20.6640625" style="15" customWidth="1"/>
+    <col min="7" max="7" width="42.5" style="15" customWidth="1"/>
+    <col min="8" max="8" width="3" style="15" customWidth="1"/>
+    <col min="9" max="9" width="44" style="15" customWidth="1"/>
+    <col min="10" max="10" width="27.33203125" style="15" customWidth="1"/>
+    <col min="11" max="11" width="17.5" style="15" customWidth="1"/>
+    <col min="12" max="12" width="13.33203125" style="15" customWidth="1"/>
+    <col min="13" max="13" width="27.6640625" style="15" customWidth="1"/>
+    <col min="14" max="14" width="2.5" style="21" customWidth="1"/>
+    <col min="15" max="15" width="19.5" style="15" customWidth="1"/>
+    <col min="16" max="16" width="18.83203125" style="15" customWidth="1"/>
+    <col min="17" max="17" width="14" style="15" customWidth="1"/>
+    <col min="18" max="18" width="15.33203125" style="15" customWidth="1"/>
+    <col min="19" max="19" width="8" style="15" customWidth="1"/>
+    <col min="20" max="20" width="28.1640625" style="15" customWidth="1"/>
+    <col min="21" max="263" width="9.1640625" style="15"/>
+    <col min="264" max="264" width="15.5" style="15" customWidth="1"/>
+    <col min="265" max="265" width="27.83203125" style="15" customWidth="1"/>
+    <col min="266" max="266" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="267" max="267" width="33.1640625" style="15" customWidth="1"/>
+    <col min="268" max="268" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="9.1640625" style="15"/>
+    <col min="270" max="270" width="17.83203125" style="15" customWidth="1"/>
+    <col min="271" max="519" width="9.1640625" style="15"/>
+    <col min="520" max="520" width="15.5" style="15" customWidth="1"/>
+    <col min="521" max="521" width="27.83203125" style="15" customWidth="1"/>
+    <col min="522" max="522" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="523" max="523" width="33.1640625" style="15" customWidth="1"/>
+    <col min="524" max="524" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="525" max="525" width="9.1640625" style="15"/>
+    <col min="526" max="526" width="17.83203125" style="15" customWidth="1"/>
+    <col min="527" max="775" width="9.1640625" style="15"/>
+    <col min="776" max="776" width="15.5" style="15" customWidth="1"/>
+    <col min="777" max="777" width="27.83203125" style="15" customWidth="1"/>
+    <col min="778" max="778" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="779" max="779" width="33.1640625" style="15" customWidth="1"/>
+    <col min="780" max="780" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="781" max="781" width="9.1640625" style="15"/>
+    <col min="782" max="782" width="17.83203125" style="15" customWidth="1"/>
+    <col min="783" max="1031" width="9.1640625" style="15"/>
+    <col min="1032" max="1032" width="15.5" style="15" customWidth="1"/>
+    <col min="1033" max="1033" width="27.83203125" style="15" customWidth="1"/>
+    <col min="1034" max="1034" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="1035" max="1035" width="33.1640625" style="15" customWidth="1"/>
+    <col min="1036" max="1036" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="1037" max="1037" width="9.1640625" style="15"/>
+    <col min="1038" max="1038" width="17.83203125" style="15" customWidth="1"/>
+    <col min="1039" max="1287" width="9.1640625" style="15"/>
+    <col min="1288" max="1288" width="15.5" style="15" customWidth="1"/>
+    <col min="1289" max="1289" width="27.83203125" style="15" customWidth="1"/>
+    <col min="1290" max="1290" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="1291" max="1291" width="33.1640625" style="15" customWidth="1"/>
+    <col min="1292" max="1292" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="1293" max="1293" width="9.1640625" style="15"/>
+    <col min="1294" max="1294" width="17.83203125" style="15" customWidth="1"/>
+    <col min="1295" max="1543" width="9.1640625" style="15"/>
+    <col min="1544" max="1544" width="15.5" style="15" customWidth="1"/>
+    <col min="1545" max="1545" width="27.83203125" style="15" customWidth="1"/>
+    <col min="1546" max="1546" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="1547" max="1547" width="33.1640625" style="15" customWidth="1"/>
+    <col min="1548" max="1548" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="1549" max="1549" width="9.1640625" style="15"/>
+    <col min="1550" max="1550" width="17.83203125" style="15" customWidth="1"/>
+    <col min="1551" max="1799" width="9.1640625" style="15"/>
+    <col min="1800" max="1800" width="15.5" style="15" customWidth="1"/>
+    <col min="1801" max="1801" width="27.83203125" style="15" customWidth="1"/>
+    <col min="1802" max="1802" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="1803" max="1803" width="33.1640625" style="15" customWidth="1"/>
+    <col min="1804" max="1804" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="1805" max="1805" width="9.1640625" style="15"/>
+    <col min="1806" max="1806" width="17.83203125" style="15" customWidth="1"/>
+    <col min="1807" max="2055" width="9.1640625" style="15"/>
+    <col min="2056" max="2056" width="15.5" style="15" customWidth="1"/>
+    <col min="2057" max="2057" width="27.83203125" style="15" customWidth="1"/>
+    <col min="2058" max="2058" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="2059" max="2059" width="33.1640625" style="15" customWidth="1"/>
+    <col min="2060" max="2060" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="2061" max="2061" width="9.1640625" style="15"/>
+    <col min="2062" max="2062" width="17.83203125" style="15" customWidth="1"/>
+    <col min="2063" max="2311" width="9.1640625" style="15"/>
+    <col min="2312" max="2312" width="15.5" style="15" customWidth="1"/>
+    <col min="2313" max="2313" width="27.83203125" style="15" customWidth="1"/>
+    <col min="2314" max="2314" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="2315" max="2315" width="33.1640625" style="15" customWidth="1"/>
+    <col min="2316" max="2316" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="2317" max="2317" width="9.1640625" style="15"/>
+    <col min="2318" max="2318" width="17.83203125" style="15" customWidth="1"/>
+    <col min="2319" max="2567" width="9.1640625" style="15"/>
+    <col min="2568" max="2568" width="15.5" style="15" customWidth="1"/>
+    <col min="2569" max="2569" width="27.83203125" style="15" customWidth="1"/>
+    <col min="2570" max="2570" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="2571" max="2571" width="33.1640625" style="15" customWidth="1"/>
+    <col min="2572" max="2572" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="2573" max="2573" width="9.1640625" style="15"/>
+    <col min="2574" max="2574" width="17.83203125" style="15" customWidth="1"/>
+    <col min="2575" max="2823" width="9.1640625" style="15"/>
+    <col min="2824" max="2824" width="15.5" style="15" customWidth="1"/>
+    <col min="2825" max="2825" width="27.83203125" style="15" customWidth="1"/>
+    <col min="2826" max="2826" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="2827" max="2827" width="33.1640625" style="15" customWidth="1"/>
+    <col min="2828" max="2828" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="2829" max="2829" width="9.1640625" style="15"/>
+    <col min="2830" max="2830" width="17.83203125" style="15" customWidth="1"/>
+    <col min="2831" max="3079" width="9.1640625" style="15"/>
+    <col min="3080" max="3080" width="15.5" style="15" customWidth="1"/>
+    <col min="3081" max="3081" width="27.83203125" style="15" customWidth="1"/>
+    <col min="3082" max="3082" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="3083" max="3083" width="33.1640625" style="15" customWidth="1"/>
+    <col min="3084" max="3084" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="3085" max="3085" width="9.1640625" style="15"/>
+    <col min="3086" max="3086" width="17.83203125" style="15" customWidth="1"/>
+    <col min="3087" max="3335" width="9.1640625" style="15"/>
+    <col min="3336" max="3336" width="15.5" style="15" customWidth="1"/>
+    <col min="3337" max="3337" width="27.83203125" style="15" customWidth="1"/>
+    <col min="3338" max="3338" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="3339" max="3339" width="33.1640625" style="15" customWidth="1"/>
+    <col min="3340" max="3340" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="3341" max="3341" width="9.1640625" style="15"/>
+    <col min="3342" max="3342" width="17.83203125" style="15" customWidth="1"/>
+    <col min="3343" max="3591" width="9.1640625" style="15"/>
+    <col min="3592" max="3592" width="15.5" style="15" customWidth="1"/>
+    <col min="3593" max="3593" width="27.83203125" style="15" customWidth="1"/>
+    <col min="3594" max="3594" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="3595" max="3595" width="33.1640625" style="15" customWidth="1"/>
+    <col min="3596" max="3596" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="3597" max="3597" width="9.1640625" style="15"/>
+    <col min="3598" max="3598" width="17.83203125" style="15" customWidth="1"/>
+    <col min="3599" max="3847" width="9.1640625" style="15"/>
+    <col min="3848" max="3848" width="15.5" style="15" customWidth="1"/>
+    <col min="3849" max="3849" width="27.83203125" style="15" customWidth="1"/>
+    <col min="3850" max="3850" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="3851" max="3851" width="33.1640625" style="15" customWidth="1"/>
+    <col min="3852" max="3852" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="3853" max="3853" width="9.1640625" style="15"/>
+    <col min="3854" max="3854" width="17.83203125" style="15" customWidth="1"/>
+    <col min="3855" max="4103" width="9.1640625" style="15"/>
+    <col min="4104" max="4104" width="15.5" style="15" customWidth="1"/>
+    <col min="4105" max="4105" width="27.83203125" style="15" customWidth="1"/>
+    <col min="4106" max="4106" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="4107" max="4107" width="33.1640625" style="15" customWidth="1"/>
+    <col min="4108" max="4108" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="4109" max="4109" width="9.1640625" style="15"/>
+    <col min="4110" max="4110" width="17.83203125" style="15" customWidth="1"/>
+    <col min="4111" max="4359" width="9.1640625" style="15"/>
+    <col min="4360" max="4360" width="15.5" style="15" customWidth="1"/>
+    <col min="4361" max="4361" width="27.83203125" style="15" customWidth="1"/>
+    <col min="4362" max="4362" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="4363" max="4363" width="33.1640625" style="15" customWidth="1"/>
+    <col min="4364" max="4364" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="4365" max="4365" width="9.1640625" style="15"/>
+    <col min="4366" max="4366" width="17.83203125" style="15" customWidth="1"/>
+    <col min="4367" max="4615" width="9.1640625" style="15"/>
+    <col min="4616" max="4616" width="15.5" style="15" customWidth="1"/>
+    <col min="4617" max="4617" width="27.83203125" style="15" customWidth="1"/>
+    <col min="4618" max="4618" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="4619" max="4619" width="33.1640625" style="15" customWidth="1"/>
+    <col min="4620" max="4620" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="4621" max="4621" width="9.1640625" style="15"/>
+    <col min="4622" max="4622" width="17.83203125" style="15" customWidth="1"/>
+    <col min="4623" max="4871" width="9.1640625" style="15"/>
+    <col min="4872" max="4872" width="15.5" style="15" customWidth="1"/>
+    <col min="4873" max="4873" width="27.83203125" style="15" customWidth="1"/>
+    <col min="4874" max="4874" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="4875" max="4875" width="33.1640625" style="15" customWidth="1"/>
+    <col min="4876" max="4876" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="4877" max="4877" width="9.1640625" style="15"/>
+    <col min="4878" max="4878" width="17.83203125" style="15" customWidth="1"/>
+    <col min="4879" max="5127" width="9.1640625" style="15"/>
+    <col min="5128" max="5128" width="15.5" style="15" customWidth="1"/>
+    <col min="5129" max="5129" width="27.83203125" style="15" customWidth="1"/>
+    <col min="5130" max="5130" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="5131" max="5131" width="33.1640625" style="15" customWidth="1"/>
+    <col min="5132" max="5132" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="5133" max="5133" width="9.1640625" style="15"/>
+    <col min="5134" max="5134" width="17.83203125" style="15" customWidth="1"/>
+    <col min="5135" max="5383" width="9.1640625" style="15"/>
+    <col min="5384" max="5384" width="15.5" style="15" customWidth="1"/>
+    <col min="5385" max="5385" width="27.83203125" style="15" customWidth="1"/>
+    <col min="5386" max="5386" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="5387" max="5387" width="33.1640625" style="15" customWidth="1"/>
+    <col min="5388" max="5388" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="5389" max="5389" width="9.1640625" style="15"/>
+    <col min="5390" max="5390" width="17.83203125" style="15" customWidth="1"/>
+    <col min="5391" max="5639" width="9.1640625" style="15"/>
+    <col min="5640" max="5640" width="15.5" style="15" customWidth="1"/>
+    <col min="5641" max="5641" width="27.83203125" style="15" customWidth="1"/>
+    <col min="5642" max="5642" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="5643" max="5643" width="33.1640625" style="15" customWidth="1"/>
+    <col min="5644" max="5644" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="5645" max="5645" width="9.1640625" style="15"/>
+    <col min="5646" max="5646" width="17.83203125" style="15" customWidth="1"/>
+    <col min="5647" max="5895" width="9.1640625" style="15"/>
+    <col min="5896" max="5896" width="15.5" style="15" customWidth="1"/>
+    <col min="5897" max="5897" width="27.83203125" style="15" customWidth="1"/>
+    <col min="5898" max="5898" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="5899" max="5899" width="33.1640625" style="15" customWidth="1"/>
+    <col min="5900" max="5900" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="5901" max="5901" width="9.1640625" style="15"/>
+    <col min="5902" max="5902" width="17.83203125" style="15" customWidth="1"/>
+    <col min="5903" max="6151" width="9.1640625" style="15"/>
+    <col min="6152" max="6152" width="15.5" style="15" customWidth="1"/>
+    <col min="6153" max="6153" width="27.83203125" style="15" customWidth="1"/>
+    <col min="6154" max="6154" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="6155" max="6155" width="33.1640625" style="15" customWidth="1"/>
+    <col min="6156" max="6156" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="6157" max="6157" width="9.1640625" style="15"/>
+    <col min="6158" max="6158" width="17.83203125" style="15" customWidth="1"/>
+    <col min="6159" max="6407" width="9.1640625" style="15"/>
+    <col min="6408" max="6408" width="15.5" style="15" customWidth="1"/>
+    <col min="6409" max="6409" width="27.83203125" style="15" customWidth="1"/>
+    <col min="6410" max="6410" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="6411" max="6411" width="33.1640625" style="15" customWidth="1"/>
+    <col min="6412" max="6412" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="6413" max="6413" width="9.1640625" style="15"/>
+    <col min="6414" max="6414" width="17.83203125" style="15" customWidth="1"/>
+    <col min="6415" max="6663" width="9.1640625" style="15"/>
+    <col min="6664" max="6664" width="15.5" style="15" customWidth="1"/>
+    <col min="6665" max="6665" width="27.83203125" style="15" customWidth="1"/>
+    <col min="6666" max="6666" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="6667" max="6667" width="33.1640625" style="15" customWidth="1"/>
+    <col min="6668" max="6668" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="6669" max="6669" width="9.1640625" style="15"/>
+    <col min="6670" max="6670" width="17.83203125" style="15" customWidth="1"/>
+    <col min="6671" max="6919" width="9.1640625" style="15"/>
+    <col min="6920" max="6920" width="15.5" style="15" customWidth="1"/>
+    <col min="6921" max="6921" width="27.83203125" style="15" customWidth="1"/>
+    <col min="6922" max="6922" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="6923" max="6923" width="33.1640625" style="15" customWidth="1"/>
+    <col min="6924" max="6924" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="6925" max="6925" width="9.1640625" style="15"/>
+    <col min="6926" max="6926" width="17.83203125" style="15" customWidth="1"/>
+    <col min="6927" max="7175" width="9.1640625" style="15"/>
+    <col min="7176" max="7176" width="15.5" style="15" customWidth="1"/>
+    <col min="7177" max="7177" width="27.83203125" style="15" customWidth="1"/>
+    <col min="7178" max="7178" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="7179" max="7179" width="33.1640625" style="15" customWidth="1"/>
+    <col min="7180" max="7180" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="7181" max="7181" width="9.1640625" style="15"/>
+    <col min="7182" max="7182" width="17.83203125" style="15" customWidth="1"/>
+    <col min="7183" max="7431" width="9.1640625" style="15"/>
+    <col min="7432" max="7432" width="15.5" style="15" customWidth="1"/>
+    <col min="7433" max="7433" width="27.83203125" style="15" customWidth="1"/>
+    <col min="7434" max="7434" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="7435" max="7435" width="33.1640625" style="15" customWidth="1"/>
+    <col min="7436" max="7436" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="7437" max="7437" width="9.1640625" style="15"/>
+    <col min="7438" max="7438" width="17.83203125" style="15" customWidth="1"/>
+    <col min="7439" max="7687" width="9.1640625" style="15"/>
+    <col min="7688" max="7688" width="15.5" style="15" customWidth="1"/>
+    <col min="7689" max="7689" width="27.83203125" style="15" customWidth="1"/>
+    <col min="7690" max="7690" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="7691" max="7691" width="33.1640625" style="15" customWidth="1"/>
+    <col min="7692" max="7692" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="7693" max="7693" width="9.1640625" style="15"/>
+    <col min="7694" max="7694" width="17.83203125" style="15" customWidth="1"/>
+    <col min="7695" max="7943" width="9.1640625" style="15"/>
+    <col min="7944" max="7944" width="15.5" style="15" customWidth="1"/>
+    <col min="7945" max="7945" width="27.83203125" style="15" customWidth="1"/>
+    <col min="7946" max="7946" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="7947" max="7947" width="33.1640625" style="15" customWidth="1"/>
+    <col min="7948" max="7948" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="7949" max="7949" width="9.1640625" style="15"/>
+    <col min="7950" max="7950" width="17.83203125" style="15" customWidth="1"/>
+    <col min="7951" max="8199" width="9.1640625" style="15"/>
+    <col min="8200" max="8200" width="15.5" style="15" customWidth="1"/>
+    <col min="8201" max="8201" width="27.83203125" style="15" customWidth="1"/>
+    <col min="8202" max="8202" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="8203" max="8203" width="33.1640625" style="15" customWidth="1"/>
+    <col min="8204" max="8204" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="8205" max="8205" width="9.1640625" style="15"/>
+    <col min="8206" max="8206" width="17.83203125" style="15" customWidth="1"/>
+    <col min="8207" max="8455" width="9.1640625" style="15"/>
+    <col min="8456" max="8456" width="15.5" style="15" customWidth="1"/>
+    <col min="8457" max="8457" width="27.83203125" style="15" customWidth="1"/>
+    <col min="8458" max="8458" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="8459" max="8459" width="33.1640625" style="15" customWidth="1"/>
+    <col min="8460" max="8460" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="8461" max="8461" width="9.1640625" style="15"/>
+    <col min="8462" max="8462" width="17.83203125" style="15" customWidth="1"/>
+    <col min="8463" max="8711" width="9.1640625" style="15"/>
+    <col min="8712" max="8712" width="15.5" style="15" customWidth="1"/>
+    <col min="8713" max="8713" width="27.83203125" style="15" customWidth="1"/>
+    <col min="8714" max="8714" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="8715" max="8715" width="33.1640625" style="15" customWidth="1"/>
+    <col min="8716" max="8716" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="8717" max="8717" width="9.1640625" style="15"/>
+    <col min="8718" max="8718" width="17.83203125" style="15" customWidth="1"/>
+    <col min="8719" max="8967" width="9.1640625" style="15"/>
+    <col min="8968" max="8968" width="15.5" style="15" customWidth="1"/>
+    <col min="8969" max="8969" width="27.83203125" style="15" customWidth="1"/>
+    <col min="8970" max="8970" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="8971" max="8971" width="33.1640625" style="15" customWidth="1"/>
+    <col min="8972" max="8972" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="8973" max="8973" width="9.1640625" style="15"/>
+    <col min="8974" max="8974" width="17.83203125" style="15" customWidth="1"/>
+    <col min="8975" max="9223" width="9.1640625" style="15"/>
+    <col min="9224" max="9224" width="15.5" style="15" customWidth="1"/>
+    <col min="9225" max="9225" width="27.83203125" style="15" customWidth="1"/>
+    <col min="9226" max="9226" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="9227" max="9227" width="33.1640625" style="15" customWidth="1"/>
+    <col min="9228" max="9228" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="9229" max="9229" width="9.1640625" style="15"/>
+    <col min="9230" max="9230" width="17.83203125" style="15" customWidth="1"/>
+    <col min="9231" max="9479" width="9.1640625" style="15"/>
+    <col min="9480" max="9480" width="15.5" style="15" customWidth="1"/>
+    <col min="9481" max="9481" width="27.83203125" style="15" customWidth="1"/>
+    <col min="9482" max="9482" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="9483" max="9483" width="33.1640625" style="15" customWidth="1"/>
+    <col min="9484" max="9484" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="9485" max="9485" width="9.1640625" style="15"/>
+    <col min="9486" max="9486" width="17.83203125" style="15" customWidth="1"/>
+    <col min="9487" max="9735" width="9.1640625" style="15"/>
+    <col min="9736" max="9736" width="15.5" style="15" customWidth="1"/>
+    <col min="9737" max="9737" width="27.83203125" style="15" customWidth="1"/>
+    <col min="9738" max="9738" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="9739" max="9739" width="33.1640625" style="15" customWidth="1"/>
+    <col min="9740" max="9740" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="9741" max="9741" width="9.1640625" style="15"/>
+    <col min="9742" max="9742" width="17.83203125" style="15" customWidth="1"/>
+    <col min="9743" max="9991" width="9.1640625" style="15"/>
+    <col min="9992" max="9992" width="15.5" style="15" customWidth="1"/>
+    <col min="9993" max="9993" width="27.83203125" style="15" customWidth="1"/>
+    <col min="9994" max="9994" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="9995" max="9995" width="33.1640625" style="15" customWidth="1"/>
+    <col min="9996" max="9996" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="9997" max="9997" width="9.1640625" style="15"/>
+    <col min="9998" max="9998" width="17.83203125" style="15" customWidth="1"/>
+    <col min="9999" max="10247" width="9.1640625" style="15"/>
+    <col min="10248" max="10248" width="15.5" style="15" customWidth="1"/>
+    <col min="10249" max="10249" width="27.83203125" style="15" customWidth="1"/>
+    <col min="10250" max="10250" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="10251" max="10251" width="33.1640625" style="15" customWidth="1"/>
+    <col min="10252" max="10252" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="10253" max="10253" width="9.1640625" style="15"/>
+    <col min="10254" max="10254" width="17.83203125" style="15" customWidth="1"/>
+    <col min="10255" max="10503" width="9.1640625" style="15"/>
+    <col min="10504" max="10504" width="15.5" style="15" customWidth="1"/>
+    <col min="10505" max="10505" width="27.83203125" style="15" customWidth="1"/>
+    <col min="10506" max="10506" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="10507" max="10507" width="33.1640625" style="15" customWidth="1"/>
+    <col min="10508" max="10508" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="10509" max="10509" width="9.1640625" style="15"/>
+    <col min="10510" max="10510" width="17.83203125" style="15" customWidth="1"/>
+    <col min="10511" max="10759" width="9.1640625" style="15"/>
+    <col min="10760" max="10760" width="15.5" style="15" customWidth="1"/>
+    <col min="10761" max="10761" width="27.83203125" style="15" customWidth="1"/>
+    <col min="10762" max="10762" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="10763" max="10763" width="33.1640625" style="15" customWidth="1"/>
+    <col min="10764" max="10764" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="10765" max="10765" width="9.1640625" style="15"/>
+    <col min="10766" max="10766" width="17.83203125" style="15" customWidth="1"/>
+    <col min="10767" max="11015" width="9.1640625" style="15"/>
+    <col min="11016" max="11016" width="15.5" style="15" customWidth="1"/>
+    <col min="11017" max="11017" width="27.83203125" style="15" customWidth="1"/>
+    <col min="11018" max="11018" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="11019" max="11019" width="33.1640625" style="15" customWidth="1"/>
+    <col min="11020" max="11020" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="11021" max="11021" width="9.1640625" style="15"/>
+    <col min="11022" max="11022" width="17.83203125" style="15" customWidth="1"/>
+    <col min="11023" max="11271" width="9.1640625" style="15"/>
+    <col min="11272" max="11272" width="15.5" style="15" customWidth="1"/>
+    <col min="11273" max="11273" width="27.83203125" style="15" customWidth="1"/>
+    <col min="11274" max="11274" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="11275" max="11275" width="33.1640625" style="15" customWidth="1"/>
+    <col min="11276" max="11276" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="11277" max="11277" width="9.1640625" style="15"/>
+    <col min="11278" max="11278" width="17.83203125" style="15" customWidth="1"/>
+    <col min="11279" max="11527" width="9.1640625" style="15"/>
+    <col min="11528" max="11528" width="15.5" style="15" customWidth="1"/>
+    <col min="11529" max="11529" width="27.83203125" style="15" customWidth="1"/>
+    <col min="11530" max="11530" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="11531" max="11531" width="33.1640625" style="15" customWidth="1"/>
+    <col min="11532" max="11532" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="11533" max="11533" width="9.1640625" style="15"/>
+    <col min="11534" max="11534" width="17.83203125" style="15" customWidth="1"/>
+    <col min="11535" max="11783" width="9.1640625" style="15"/>
+    <col min="11784" max="11784" width="15.5" style="15" customWidth="1"/>
+    <col min="11785" max="11785" width="27.83203125" style="15" customWidth="1"/>
+    <col min="11786" max="11786" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="11787" max="11787" width="33.1640625" style="15" customWidth="1"/>
+    <col min="11788" max="11788" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="11789" max="11789" width="9.1640625" style="15"/>
+    <col min="11790" max="11790" width="17.83203125" style="15" customWidth="1"/>
+    <col min="11791" max="12039" width="9.1640625" style="15"/>
+    <col min="12040" max="12040" width="15.5" style="15" customWidth="1"/>
+    <col min="12041" max="12041" width="27.83203125" style="15" customWidth="1"/>
+    <col min="12042" max="12042" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="12043" max="12043" width="33.1640625" style="15" customWidth="1"/>
+    <col min="12044" max="12044" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="12045" max="12045" width="9.1640625" style="15"/>
+    <col min="12046" max="12046" width="17.83203125" style="15" customWidth="1"/>
+    <col min="12047" max="12295" width="9.1640625" style="15"/>
+    <col min="12296" max="12296" width="15.5" style="15" customWidth="1"/>
+    <col min="12297" max="12297" width="27.83203125" style="15" customWidth="1"/>
+    <col min="12298" max="12298" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="12299" max="12299" width="33.1640625" style="15" customWidth="1"/>
+    <col min="12300" max="12300" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="12301" max="12301" width="9.1640625" style="15"/>
+    <col min="12302" max="12302" width="17.83203125" style="15" customWidth="1"/>
+    <col min="12303" max="12551" width="9.1640625" style="15"/>
+    <col min="12552" max="12552" width="15.5" style="15" customWidth="1"/>
+    <col min="12553" max="12553" width="27.83203125" style="15" customWidth="1"/>
+    <col min="12554" max="12554" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="12555" max="12555" width="33.1640625" style="15" customWidth="1"/>
+    <col min="12556" max="12556" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="12557" max="12557" width="9.1640625" style="15"/>
+    <col min="12558" max="12558" width="17.83203125" style="15" customWidth="1"/>
+    <col min="12559" max="12807" width="9.1640625" style="15"/>
+    <col min="12808" max="12808" width="15.5" style="15" customWidth="1"/>
+    <col min="12809" max="12809" width="27.83203125" style="15" customWidth="1"/>
+    <col min="12810" max="12810" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="12811" max="12811" width="33.1640625" style="15" customWidth="1"/>
+    <col min="12812" max="12812" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="12813" max="12813" width="9.1640625" style="15"/>
+    <col min="12814" max="12814" width="17.83203125" style="15" customWidth="1"/>
+    <col min="12815" max="13063" width="9.1640625" style="15"/>
+    <col min="13064" max="13064" width="15.5" style="15" customWidth="1"/>
+    <col min="13065" max="13065" width="27.83203125" style="15" customWidth="1"/>
+    <col min="13066" max="13066" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="13067" max="13067" width="33.1640625" style="15" customWidth="1"/>
+    <col min="13068" max="13068" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="13069" max="13069" width="9.1640625" style="15"/>
+    <col min="13070" max="13070" width="17.83203125" style="15" customWidth="1"/>
+    <col min="13071" max="13319" width="9.1640625" style="15"/>
+    <col min="13320" max="13320" width="15.5" style="15" customWidth="1"/>
+    <col min="13321" max="13321" width="27.83203125" style="15" customWidth="1"/>
+    <col min="13322" max="13322" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="13323" max="13323" width="33.1640625" style="15" customWidth="1"/>
+    <col min="13324" max="13324" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="13325" max="13325" width="9.1640625" style="15"/>
+    <col min="13326" max="13326" width="17.83203125" style="15" customWidth="1"/>
+    <col min="13327" max="13575" width="9.1640625" style="15"/>
+    <col min="13576" max="13576" width="15.5" style="15" customWidth="1"/>
+    <col min="13577" max="13577" width="27.83203125" style="15" customWidth="1"/>
+    <col min="13578" max="13578" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="13579" max="13579" width="33.1640625" style="15" customWidth="1"/>
+    <col min="13580" max="13580" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="13581" max="13581" width="9.1640625" style="15"/>
+    <col min="13582" max="13582" width="17.83203125" style="15" customWidth="1"/>
+    <col min="13583" max="13831" width="9.1640625" style="15"/>
+    <col min="13832" max="13832" width="15.5" style="15" customWidth="1"/>
+    <col min="13833" max="13833" width="27.83203125" style="15" customWidth="1"/>
+    <col min="13834" max="13834" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="13835" max="13835" width="33.1640625" style="15" customWidth="1"/>
+    <col min="13836" max="13836" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="13837" max="13837" width="9.1640625" style="15"/>
+    <col min="13838" max="13838" width="17.83203125" style="15" customWidth="1"/>
+    <col min="13839" max="14087" width="9.1640625" style="15"/>
+    <col min="14088" max="14088" width="15.5" style="15" customWidth="1"/>
+    <col min="14089" max="14089" width="27.83203125" style="15" customWidth="1"/>
+    <col min="14090" max="14090" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="14091" max="14091" width="33.1640625" style="15" customWidth="1"/>
+    <col min="14092" max="14092" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="14093" max="14093" width="9.1640625" style="15"/>
+    <col min="14094" max="14094" width="17.83203125" style="15" customWidth="1"/>
+    <col min="14095" max="14343" width="9.1640625" style="15"/>
+    <col min="14344" max="14344" width="15.5" style="15" customWidth="1"/>
+    <col min="14345" max="14345" width="27.83203125" style="15" customWidth="1"/>
+    <col min="14346" max="14346" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="14347" max="14347" width="33.1640625" style="15" customWidth="1"/>
+    <col min="14348" max="14348" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="14349" max="14349" width="9.1640625" style="15"/>
+    <col min="14350" max="14350" width="17.83203125" style="15" customWidth="1"/>
+    <col min="14351" max="14599" width="9.1640625" style="15"/>
+    <col min="14600" max="14600" width="15.5" style="15" customWidth="1"/>
+    <col min="14601" max="14601" width="27.83203125" style="15" customWidth="1"/>
+    <col min="14602" max="14602" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="14603" max="14603" width="33.1640625" style="15" customWidth="1"/>
+    <col min="14604" max="14604" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="14605" max="14605" width="9.1640625" style="15"/>
+    <col min="14606" max="14606" width="17.83203125" style="15" customWidth="1"/>
+    <col min="14607" max="14855" width="9.1640625" style="15"/>
+    <col min="14856" max="14856" width="15.5" style="15" customWidth="1"/>
+    <col min="14857" max="14857" width="27.83203125" style="15" customWidth="1"/>
+    <col min="14858" max="14858" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="14859" max="14859" width="33.1640625" style="15" customWidth="1"/>
+    <col min="14860" max="14860" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="14861" max="14861" width="9.1640625" style="15"/>
+    <col min="14862" max="14862" width="17.83203125" style="15" customWidth="1"/>
+    <col min="14863" max="15111" width="9.1640625" style="15"/>
+    <col min="15112" max="15112" width="15.5" style="15" customWidth="1"/>
+    <col min="15113" max="15113" width="27.83203125" style="15" customWidth="1"/>
+    <col min="15114" max="15114" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="15115" max="15115" width="33.1640625" style="15" customWidth="1"/>
+    <col min="15116" max="15116" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="15117" max="15117" width="9.1640625" style="15"/>
+    <col min="15118" max="15118" width="17.83203125" style="15" customWidth="1"/>
+    <col min="15119" max="15367" width="9.1640625" style="15"/>
+    <col min="15368" max="15368" width="15.5" style="15" customWidth="1"/>
+    <col min="15369" max="15369" width="27.83203125" style="15" customWidth="1"/>
+    <col min="15370" max="15370" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="15371" max="15371" width="33.1640625" style="15" customWidth="1"/>
+    <col min="15372" max="15372" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="15373" max="15373" width="9.1640625" style="15"/>
+    <col min="15374" max="15374" width="17.83203125" style="15" customWidth="1"/>
+    <col min="15375" max="15623" width="9.1640625" style="15"/>
+    <col min="15624" max="15624" width="15.5" style="15" customWidth="1"/>
+    <col min="15625" max="15625" width="27.83203125" style="15" customWidth="1"/>
+    <col min="15626" max="15626" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="15627" max="15627" width="33.1640625" style="15" customWidth="1"/>
+    <col min="15628" max="15628" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="15629" max="15629" width="9.1640625" style="15"/>
+    <col min="15630" max="15630" width="17.83203125" style="15" customWidth="1"/>
+    <col min="15631" max="15879" width="9.1640625" style="15"/>
+    <col min="15880" max="15880" width="15.5" style="15" customWidth="1"/>
+    <col min="15881" max="15881" width="27.83203125" style="15" customWidth="1"/>
+    <col min="15882" max="15882" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="15883" max="15883" width="33.1640625" style="15" customWidth="1"/>
+    <col min="15884" max="15884" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="15885" max="15885" width="9.1640625" style="15"/>
+    <col min="15886" max="15886" width="17.83203125" style="15" customWidth="1"/>
+    <col min="15887" max="16135" width="9.1640625" style="15"/>
+    <col min="16136" max="16136" width="15.5" style="15" customWidth="1"/>
+    <col min="16137" max="16137" width="27.83203125" style="15" customWidth="1"/>
+    <col min="16138" max="16138" width="68" style="15" bestFit="1" customWidth="1"/>
+    <col min="16139" max="16139" width="33.1640625" style="15" customWidth="1"/>
+    <col min="16140" max="16140" width="8" style="15" bestFit="1" customWidth="1"/>
+    <col min="16141" max="16141" width="9.1640625" style="15"/>
+    <col min="16142" max="16142" width="17.83203125" style="15" customWidth="1"/>
+    <col min="16143" max="16384" width="9.1640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:68" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="135" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:68" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="135" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="136"/>
-      <c r="D2" s="136"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="136"/>
+      <c r="G2" s="136"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="20" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B3" s="137" t="s">
+    <row r="3" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E3" s="151" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="149"/>
-      <c r="D3" s="138"/>
-      <c r="E3" s="17"/>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B4" s="119"/>
-      <c r="C4" s="150"/>
-      <c r="D4" s="83" t="s">
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="17"/>
+      <c r="I3" s="14"/>
+    </row>
+    <row r="4" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E4" s="119"/>
+      <c r="F4" s="147"/>
+      <c r="G4" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="E4" s="17"/>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B5" s="137" t="s">
+      <c r="H4" s="17"/>
+      <c r="I4" s="14"/>
+    </row>
+    <row r="5" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E5" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="149"/>
-      <c r="D5" s="138"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="18"/>
-    </row>
-    <row r="6" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="139" t="s">
+      <c r="F5" s="146"/>
+      <c r="G5" s="146"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="18"/>
+    </row>
+    <row r="6" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E6" s="138" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="151"/>
-      <c r="D6" s="140"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="18"/>
-    </row>
-    <row r="7" spans="1:65" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="121"/>
-      <c r="C7" s="152"/>
-      <c r="D7" s="120" t="s">
+      <c r="F6" s="148"/>
+      <c r="G6" s="148"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+    </row>
+    <row r="7" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E7" s="121"/>
+      <c r="F7" s="149"/>
+      <c r="G7" s="120" t="s">
         <v>42</v>
       </c>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-    </row>
-    <row r="8" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B8" s="144" t="s">
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+    </row>
+    <row r="8" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E8" s="142" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="153"/>
-      <c r="D8" s="145"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-    </row>
-    <row r="9" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B9" s="144" t="s">
+      <c r="F8" s="150"/>
+      <c r="G8" s="150"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+    </row>
+    <row r="9" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E9" s="142" t="s">
         <v>44</v>
       </c>
-      <c r="C9" s="153"/>
-      <c r="D9" s="145"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="18"/>
-    </row>
-    <row r="10" spans="1:65" x14ac:dyDescent="0.15">
-      <c r="B10" s="144" t="s">
+      <c r="F9" s="150"/>
+      <c r="G9" s="150"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+    </row>
+    <row r="10" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="E10" s="142" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="153"/>
-      <c r="D10" s="145"/>
-      <c r="E10" s="17"/>
-      <c r="F10" s="18"/>
-    </row>
-    <row r="11" spans="1:65" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="F10" s="150"/>
+      <c r="G10" s="150"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="18"/>
+    </row>
+    <row r="11" spans="1:68" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1"/>
-      <c r="B11" s="142" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+      <c r="E11" s="140" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="143"/>
-      <c r="D11" s="143"/>
-      <c r="E11" s="13"/>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="1:65" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="141"/>
+      <c r="G11" s="141"/>
+      <c r="H11" s="13"/>
+      <c r="I11" s="14"/>
+    </row>
+    <row r="12" spans="1:68" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="96"/>
+      <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="24"/>
-      <c r="L12" s="141" t="s">
+      <c r="J12" s="96"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="24"/>
+      <c r="O12" s="139" t="s">
         <v>47</v>
       </c>
-      <c r="M12" s="141"/>
-      <c r="N12" s="141"/>
-      <c r="O12" s="141"/>
-      <c r="P12" s="141"/>
-      <c r="Q12" s="141"/>
-    </row>
-    <row r="13" spans="1:65" s="19" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="P12" s="139"/>
+      <c r="Q12" s="139"/>
+      <c r="R12" s="139"/>
+      <c r="S12" s="139"/>
+      <c r="T12" s="139"/>
+    </row>
+    <row r="13" spans="1:68" s="19" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72" t="s">
         <v>48</v>
       </c>
       <c r="B13" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" s="72" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="72" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="F13" s="72" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="98" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="98" t="s">
+      <c r="H13" s="72"/>
+      <c r="I13" s="72" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72" t="s">
+      <c r="J13" s="99" t="s">
         <v>51</v>
       </c>
-      <c r="G13" s="99" t="s">
+      <c r="K13" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="H13" s="72" t="s">
+      <c r="L13" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="72" t="s">
+      <c r="M13" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="J13" s="72" t="s">
+      <c r="N13" s="25"/>
+      <c r="O13" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="K13" s="25"/>
-      <c r="L13" s="72" t="s">
+      <c r="P13" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="M13" s="72" t="s">
+      <c r="Q13" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="N13" s="72" t="s">
+      <c r="R13" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="O13" s="72" t="s">
+      <c r="S13" s="72" t="s">
+        <v>53</v>
+      </c>
+      <c r="T13" s="111" t="s">
         <v>59</v>
       </c>
-      <c r="P13" s="72" t="s">
-        <v>54</v>
-      </c>
-      <c r="Q13" s="111" t="s">
-        <v>60</v>
-      </c>
-      <c r="R13" s="110"/>
-      <c r="S13" s="110"/>
-      <c r="T13" s="110"/>
       <c r="U13" s="110"/>
       <c r="V13" s="110"/>
       <c r="W13" s="110"/>
@@ -7467,358 +7495,395 @@
       <c r="BK13" s="110"/>
       <c r="BL13" s="110"/>
       <c r="BM13" s="110"/>
-    </row>
-    <row r="14" spans="1:65" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="133" t="s">
-        <v>61</v>
-      </c>
-      <c r="B14" s="108" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="108"/>
-      <c r="D14" s="77"/>
-      <c r="E14" s="77"/>
-      <c r="F14" s="73"/>
-      <c r="G14" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H14" s="78"/>
-      <c r="I14" s="79"/>
-      <c r="J14" s="80"/>
-      <c r="K14" s="74"/>
-      <c r="L14" s="73"/>
-      <c r="M14" s="75"/>
-      <c r="N14" s="75"/>
-      <c r="O14" s="78"/>
-      <c r="P14" s="79"/>
-      <c r="Q14" s="80"/>
-    </row>
-    <row r="15" spans="1:65" s="84" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="133"/>
-      <c r="B15" s="108" t="s">
-        <v>64</v>
-      </c>
-      <c r="C15" s="108"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="73"/>
-      <c r="G15" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H15" s="78"/>
-      <c r="I15" s="79"/>
-      <c r="J15" s="80"/>
-      <c r="K15" s="74"/>
-      <c r="L15" s="73"/>
-      <c r="M15" s="75"/>
-      <c r="N15" s="75"/>
-      <c r="O15" s="78"/>
-      <c r="P15" s="79"/>
-      <c r="Q15" s="80"/>
-    </row>
-    <row r="16" spans="1:65" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="133"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
+      <c r="BN13" s="110"/>
+      <c r="BO13" s="110"/>
+      <c r="BP13" s="110"/>
+    </row>
+    <row r="14" spans="1:68" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="109"/>
+      <c r="B14" s="122"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="108"/>
+      <c r="F14" s="108"/>
+      <c r="G14" s="77"/>
+      <c r="H14" s="77"/>
+      <c r="I14" s="73"/>
+      <c r="J14" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K14" s="78"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="80"/>
+      <c r="N14" s="74"/>
+      <c r="O14" s="73"/>
+      <c r="P14" s="75"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="78"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="80"/>
+    </row>
+    <row r="15" spans="1:68" s="84" customFormat="1" ht="13" x14ac:dyDescent="0.2">
+      <c r="A15" s="109"/>
+      <c r="B15" s="122"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="122"/>
+      <c r="E15" s="108"/>
+      <c r="F15" s="108"/>
+      <c r="G15" s="76"/>
+      <c r="H15" s="76"/>
+      <c r="I15" s="73"/>
+      <c r="J15" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K15" s="78"/>
+      <c r="L15" s="79"/>
+      <c r="M15" s="80"/>
+      <c r="N15" s="74"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="75"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="78"/>
+      <c r="S15" s="79"/>
+      <c r="T15" s="80"/>
+    </row>
+    <row r="16" spans="1:68" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="109"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="122"/>
       <c r="E16" s="76"/>
-      <c r="F16" s="73"/>
-      <c r="G16" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H16" s="78"/>
-      <c r="I16" s="79"/>
-      <c r="J16" s="80"/>
-      <c r="K16" s="74"/>
-      <c r="L16" s="73"/>
-      <c r="M16" s="75"/>
-      <c r="N16" s="75"/>
-      <c r="O16" s="78"/>
-      <c r="P16" s="79"/>
-      <c r="Q16" s="80"/>
-    </row>
-    <row r="17" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="133" t="s">
-        <v>65</v>
-      </c>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="73"/>
+      <c r="J16" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="78"/>
+      <c r="L16" s="79"/>
+      <c r="M16" s="80"/>
+      <c r="N16" s="74"/>
+      <c r="O16" s="73"/>
+      <c r="P16" s="75"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="78"/>
+      <c r="S16" s="79"/>
+      <c r="T16" s="80"/>
+    </row>
+    <row r="17" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="122"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="122"/>
       <c r="E17" s="76"/>
-      <c r="F17" s="73"/>
-      <c r="G17" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H17" s="78"/>
-      <c r="I17" s="79"/>
-      <c r="J17" s="80"/>
-      <c r="K17" s="74"/>
-      <c r="L17" s="73"/>
-      <c r="M17" s="75"/>
-      <c r="N17" s="75"/>
-      <c r="O17" s="78"/>
-      <c r="P17" s="79"/>
-      <c r="Q17" s="80"/>
-    </row>
-    <row r="18" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="133"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
+      <c r="F17" s="76"/>
+      <c r="G17" s="76"/>
+      <c r="H17" s="76"/>
+      <c r="I17" s="73"/>
+      <c r="J17" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K17" s="78"/>
+      <c r="L17" s="79"/>
+      <c r="M17" s="80"/>
+      <c r="N17" s="74"/>
+      <c r="O17" s="73"/>
+      <c r="P17" s="75"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="78"/>
+      <c r="S17" s="79"/>
+      <c r="T17" s="80"/>
+    </row>
+    <row r="18" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="122"/>
+      <c r="B18" s="122"/>
+      <c r="C18" s="122"/>
+      <c r="D18" s="122"/>
       <c r="E18" s="76"/>
-      <c r="F18" s="73"/>
-      <c r="G18" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" s="78"/>
-      <c r="I18" s="79"/>
-      <c r="J18" s="80"/>
-      <c r="K18" s="74"/>
-      <c r="L18" s="73"/>
-      <c r="M18" s="75"/>
-      <c r="N18" s="75"/>
-      <c r="O18" s="78"/>
-      <c r="P18" s="79"/>
-      <c r="Q18" s="80"/>
-    </row>
-    <row r="19" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="133"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="73"/>
+      <c r="J18" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K18" s="78"/>
+      <c r="L18" s="79"/>
+      <c r="M18" s="80"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="73"/>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="78"/>
+      <c r="S18" s="79"/>
+      <c r="T18" s="80"/>
+    </row>
+    <row r="19" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="122"/>
+      <c r="B19" s="122"/>
+      <c r="C19" s="122"/>
+      <c r="D19" s="122"/>
       <c r="E19" s="76"/>
-      <c r="F19" s="73"/>
-      <c r="G19" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H19" s="78"/>
-      <c r="I19" s="79"/>
-      <c r="J19" s="80"/>
-      <c r="K19" s="74"/>
-      <c r="L19" s="73"/>
-      <c r="M19" s="75"/>
-      <c r="N19" s="75"/>
-      <c r="O19" s="78"/>
-      <c r="P19" s="79"/>
-      <c r="Q19" s="80"/>
-    </row>
-    <row r="20" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="133"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
+      <c r="F19" s="76"/>
+      <c r="G19" s="76"/>
+      <c r="H19" s="76"/>
+      <c r="I19" s="73"/>
+      <c r="J19" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="78"/>
+      <c r="L19" s="79"/>
+      <c r="M19" s="80"/>
+      <c r="N19" s="74"/>
+      <c r="O19" s="73"/>
+      <c r="P19" s="75"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="78"/>
+      <c r="S19" s="79"/>
+      <c r="T19" s="80"/>
+    </row>
+    <row r="20" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="122"/>
+      <c r="B20" s="122"/>
+      <c r="C20" s="122"/>
+      <c r="D20" s="122"/>
       <c r="E20" s="76"/>
-      <c r="F20" s="73"/>
-      <c r="G20" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H20" s="78"/>
-      <c r="I20" s="79"/>
-      <c r="J20" s="80"/>
-      <c r="K20" s="74"/>
-      <c r="L20" s="73"/>
-      <c r="M20" s="75"/>
-      <c r="N20" s="75"/>
-      <c r="O20" s="78"/>
-      <c r="P20" s="79"/>
-      <c r="Q20" s="80"/>
-    </row>
-    <row r="21" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="134"/>
-      <c r="B21" s="73"/>
-      <c r="C21" s="73"/>
-      <c r="D21" s="73"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="73"/>
+      <c r="J20" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K20" s="78"/>
+      <c r="L20" s="79"/>
+      <c r="M20" s="80"/>
+      <c r="N20" s="74"/>
+      <c r="O20" s="73"/>
+      <c r="P20" s="75"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="78"/>
+      <c r="S20" s="79"/>
+      <c r="T20" s="80"/>
+    </row>
+    <row r="21" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="123"/>
+      <c r="B21" s="123"/>
+      <c r="C21" s="123"/>
+      <c r="D21" s="123"/>
       <c r="E21" s="73"/>
-      <c r="F21" s="81"/>
-      <c r="G21" s="109" t="s">
-        <v>63</v>
-      </c>
-      <c r="H21" s="79"/>
-      <c r="I21" s="80"/>
-      <c r="J21" s="73"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="75"/>
-      <c r="M21" s="78"/>
-      <c r="N21" s="78"/>
-      <c r="O21" s="79"/>
-      <c r="P21" s="80"/>
-      <c r="Q21" s="73"/>
-    </row>
-    <row r="22" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="134"/>
-      <c r="B22" s="73"/>
-      <c r="C22" s="73"/>
-      <c r="D22" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73"/>
+      <c r="H21" s="73"/>
+      <c r="I21" s="81"/>
+      <c r="J21" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K21" s="79"/>
+      <c r="L21" s="80"/>
+      <c r="M21" s="73"/>
+      <c r="N21" s="82"/>
+      <c r="O21" s="75"/>
+      <c r="P21" s="78"/>
+      <c r="Q21" s="78"/>
+      <c r="R21" s="79"/>
+      <c r="S21" s="80"/>
+      <c r="T21" s="73"/>
+    </row>
+    <row r="22" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="123"/>
+      <c r="B22" s="123"/>
+      <c r="C22" s="123"/>
+      <c r="D22" s="123"/>
       <c r="E22" s="73"/>
       <c r="F22" s="73"/>
-      <c r="G22" s="109" t="s">
-        <v>63</v>
-      </c>
+      <c r="G22" s="73"/>
       <c r="H22" s="73"/>
       <c r="I22" s="73"/>
-      <c r="J22" s="73"/>
-      <c r="K22" s="74"/>
+      <c r="J22" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" s="73"/>
       <c r="L22" s="73"/>
       <c r="M22" s="73"/>
-      <c r="N22" s="73"/>
+      <c r="N22" s="74"/>
       <c r="O22" s="73"/>
       <c r="P22" s="73"/>
       <c r="Q22" s="73"/>
-    </row>
-    <row r="23" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="134"/>
-      <c r="B23" s="73"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="73"/>
+      <c r="R22" s="73"/>
+      <c r="S22" s="73"/>
+      <c r="T22" s="73"/>
+    </row>
+    <row r="23" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="123"/>
+      <c r="B23" s="123"/>
+      <c r="C23" s="123"/>
+      <c r="D23" s="123"/>
       <c r="E23" s="73"/>
       <c r="F23" s="73"/>
-      <c r="G23" s="109" t="s">
-        <v>63</v>
-      </c>
+      <c r="G23" s="73"/>
       <c r="H23" s="73"/>
       <c r="I23" s="73"/>
-      <c r="J23" s="73"/>
-      <c r="K23" s="74"/>
+      <c r="J23" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K23" s="73"/>
       <c r="L23" s="73"/>
       <c r="M23" s="73"/>
-      <c r="N23" s="73"/>
+      <c r="N23" s="74"/>
       <c r="O23" s="73"/>
       <c r="P23" s="73"/>
       <c r="Q23" s="73"/>
-    </row>
-    <row r="24" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="134"/>
-      <c r="B24" s="73"/>
-      <c r="C24" s="73"/>
-      <c r="D24" s="73"/>
+      <c r="R23" s="73"/>
+      <c r="S23" s="73"/>
+      <c r="T23" s="73"/>
+    </row>
+    <row r="24" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="123"/>
+      <c r="B24" s="123"/>
+      <c r="C24" s="123"/>
+      <c r="D24" s="123"/>
       <c r="E24" s="73"/>
       <c r="F24" s="73"/>
-      <c r="G24" s="109" t="s">
-        <v>63</v>
-      </c>
+      <c r="G24" s="73"/>
       <c r="H24" s="73"/>
       <c r="I24" s="73"/>
-      <c r="J24" s="73"/>
-      <c r="K24" s="74"/>
+      <c r="J24" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24" s="73"/>
       <c r="L24" s="73"/>
       <c r="M24" s="73"/>
-      <c r="N24" s="73"/>
+      <c r="N24" s="74"/>
       <c r="O24" s="73"/>
       <c r="P24" s="73"/>
       <c r="Q24" s="73"/>
-    </row>
-    <row r="25" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="134"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
+      <c r="R24" s="73"/>
+      <c r="S24" s="73"/>
+      <c r="T24" s="73"/>
+    </row>
+    <row r="25" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="123"/>
+      <c r="B25" s="123"/>
+      <c r="C25" s="123"/>
+      <c r="D25" s="123"/>
       <c r="E25" s="73"/>
       <c r="F25" s="73"/>
-      <c r="G25" s="109" t="s">
-        <v>63</v>
-      </c>
+      <c r="G25" s="73"/>
       <c r="H25" s="73"/>
       <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="74"/>
+      <c r="J25" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K25" s="73"/>
       <c r="L25" s="73"/>
       <c r="M25" s="73"/>
-      <c r="N25" s="73"/>
+      <c r="N25" s="74"/>
       <c r="O25" s="73"/>
       <c r="P25" s="73"/>
       <c r="Q25" s="73"/>
-    </row>
-    <row r="26" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="134"/>
-      <c r="B26" s="73"/>
-      <c r="C26" s="73"/>
-      <c r="D26" s="73"/>
+      <c r="R25" s="73"/>
+      <c r="S25" s="73"/>
+      <c r="T25" s="73"/>
+    </row>
+    <row r="26" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="123"/>
+      <c r="B26" s="123"/>
+      <c r="C26" s="123"/>
+      <c r="D26" s="123"/>
       <c r="E26" s="73"/>
       <c r="F26" s="73"/>
-      <c r="G26" s="109" t="s">
-        <v>63</v>
-      </c>
+      <c r="G26" s="73"/>
       <c r="H26" s="73"/>
       <c r="I26" s="73"/>
-      <c r="J26" s="73"/>
-      <c r="K26" s="74"/>
+      <c r="J26" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K26" s="73"/>
       <c r="L26" s="73"/>
       <c r="M26" s="73"/>
-      <c r="N26" s="73"/>
+      <c r="N26" s="74"/>
       <c r="O26" s="73"/>
       <c r="P26" s="73"/>
       <c r="Q26" s="73"/>
-    </row>
-    <row r="27" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="134"/>
-      <c r="B27" s="73"/>
-      <c r="C27" s="73"/>
-      <c r="D27" s="73"/>
+      <c r="R26" s="73"/>
+      <c r="S26" s="73"/>
+      <c r="T26" s="73"/>
+    </row>
+    <row r="27" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="123"/>
+      <c r="B27" s="123"/>
+      <c r="C27" s="123"/>
+      <c r="D27" s="123"/>
       <c r="E27" s="73"/>
       <c r="F27" s="73"/>
-      <c r="G27" s="109" t="s">
-        <v>63</v>
-      </c>
+      <c r="G27" s="73"/>
       <c r="H27" s="73"/>
       <c r="I27" s="73"/>
-      <c r="J27" s="73"/>
-      <c r="K27" s="74"/>
+      <c r="J27" s="109" t="s">
+        <v>60</v>
+      </c>
+      <c r="K27" s="73"/>
       <c r="L27" s="73"/>
       <c r="M27" s="73"/>
-      <c r="N27" s="73"/>
+      <c r="N27" s="74"/>
       <c r="O27" s="73"/>
       <c r="P27" s="73"/>
       <c r="Q27" s="73"/>
-    </row>
-    <row r="28" spans="1:17" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K28" s="85"/>
-    </row>
-    <row r="29" spans="1:17" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K29" s="27"/>
-    </row>
-    <row r="30" spans="1:17" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K30" s="27"/>
-    </row>
-    <row r="31" spans="1:17" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K31" s="27"/>
-    </row>
-    <row r="32" spans="1:17" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K32" s="27"/>
-    </row>
-    <row r="33" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K33" s="27"/>
-    </row>
-    <row r="34" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K34" s="27"/>
-    </row>
-    <row r="35" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K35" s="27"/>
-    </row>
-    <row r="36" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K36" s="27"/>
-    </row>
-    <row r="37" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K37" s="27"/>
-    </row>
-    <row r="38" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K38" s="27"/>
-    </row>
-    <row r="39" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K39" s="27"/>
-    </row>
-    <row r="40" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K40" s="27"/>
-    </row>
-    <row r="41" spans="11:11" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="K41" s="27"/>
-    </row>
-    <row r="42" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="11:11" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+      <c r="R27" s="73"/>
+      <c r="S27" s="73"/>
+      <c r="T27" s="73"/>
+    </row>
+    <row r="28" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="N28" s="85"/>
+    </row>
+    <row r="29" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N29" s="27"/>
+    </row>
+    <row r="30" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N30" s="27"/>
+    </row>
+    <row r="31" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N31" s="27"/>
+    </row>
+    <row r="32" spans="1:20" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N32" s="27"/>
+    </row>
+    <row r="33" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N33" s="27"/>
+    </row>
+    <row r="34" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N34" s="27"/>
+    </row>
+    <row r="35" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N35" s="27"/>
+    </row>
+    <row r="36" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N36" s="27"/>
+    </row>
+    <row r="37" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N37" s="27"/>
+    </row>
+    <row r="38" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N38" s="27"/>
+    </row>
+    <row r="39" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N39" s="27"/>
+    </row>
+    <row r="40" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N40" s="27"/>
+    </row>
+    <row r="41" spans="14:14" s="26" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="N41" s="27"/>
+    </row>
+    <row r="42" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -7892,23 +7957,19 @@
     <row r="119" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="120" ht="15" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="L12:Q12"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="A14:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A27"/>
+  <mergeCells count="9">
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="E3:G3"/>
+    <mergeCell ref="E5:G5"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="O12:T12"/>
+    <mergeCell ref="E11:G11"/>
+    <mergeCell ref="E8:G8"/>
+    <mergeCell ref="E9:G9"/>
+    <mergeCell ref="E10:G10"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G13" location="'QA Tags'!A1" display="Tag for Findings " xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J13" location="'QA Tags'!A1" display="Tag for Findings " xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -7923,16 +7984,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>1</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
-                    <xdr:row>3</xdr:row>
-                    <xdr:rowOff>0</xdr:rowOff>
+                    <xdr:row>2</xdr:row>
+                    <xdr:rowOff>165100</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7945,16 +8006,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>2</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>25400</xdr:rowOff>
+                    <xdr:rowOff>12700</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -7967,13 +8028,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -7989,13 +8050,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8011,13 +8072,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8033,13 +8094,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
@@ -8055,13 +8116,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
@@ -8077,13 +8138,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8099,13 +8160,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8121,13 +8182,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8143,13 +8204,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8165,16 +8226,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>203200</xdr:rowOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -8187,13 +8248,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8209,13 +8270,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8231,13 +8292,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8253,13 +8314,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8275,13 +8336,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8297,13 +8358,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
@@ -8319,13 +8380,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
@@ -8341,13 +8402,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
@@ -8363,13 +8424,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8385,13 +8446,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8407,13 +8468,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8429,13 +8490,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8451,13 +8512,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8473,13 +8534,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>10</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8495,16 +8556,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>203200</xdr:rowOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -8517,16 +8578,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
-                    <xdr:row>10</xdr:row>
-                    <xdr:rowOff>203200</xdr:rowOff>
+                    <xdr:row>11</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -8539,13 +8600,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8561,13 +8622,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8583,13 +8644,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8605,13 +8666,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8627,13 +8688,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8649,13 +8710,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8671,13 +8732,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8693,13 +8754,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8715,13 +8776,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8737,13 +8798,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>8</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8759,13 +8820,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8781,13 +8842,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8803,13 +8864,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8825,13 +8886,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8847,13 +8908,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>7</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>9</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8869,13 +8930,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8891,13 +8952,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8913,13 +8974,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -8935,13 +8996,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8957,13 +9018,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -8979,13 +9040,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9001,13 +9062,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9023,13 +9084,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -9045,13 +9106,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -9067,13 +9128,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9089,13 +9150,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9111,13 +9172,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9133,13 +9194,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -9155,13 +9216,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -9177,13 +9238,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>177800</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>6</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
@@ -9199,13 +9260,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9221,13 +9282,13 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2844800</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>609600</xdr:colOff>
                     <xdr:row>5</xdr:row>
                     <xdr:rowOff>25400</xdr:rowOff>
@@ -9243,16 +9304,16 @@
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>2832100</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>0</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>5</xdr:col>
+                    <xdr:col>8</xdr:col>
                     <xdr:colOff>114300</xdr:colOff>
                     <xdr:row>5</xdr:row>
-                    <xdr:rowOff>76200</xdr:rowOff>
+                    <xdr:rowOff>88900</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -9269,7 +9330,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -9281,10 +9342,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="123" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="146" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="147"/>
+      <c r="A1" s="143" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="144"/>
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
       <c r="E1" s="43"/>
@@ -9292,7 +9353,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>15</v>
@@ -9300,44 +9361,44 @@
     </row>
     <row r="3" spans="1:6" ht="57" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="112" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="113" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -9364,10 +9425,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="118" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="148" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="148"/>
+      <c r="A1" s="145" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" s="145"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A2" s="114"/>
@@ -9376,37 +9437,37 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="115" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B3" s="115" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C3" s="114"/>
     </row>
     <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="116" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B4" s="114" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C4" s="114"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="116" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B5" s="117" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C5" s="114"/>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="116" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B6" s="117" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C6" s="114"/>
     </row>

</xml_diff>

<commit_message>
hide column, other fixes to match output of functions.
</commit_message>
<xml_diff>
--- a/inst/extdata/QA_Template_Coded_Analysis.xlsx
+++ b/inst/extdata/QA_Template_Coded_Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzadra41/Documents/R Projects/integral-private/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF59A3D3-D50D-0D40-AA21-6DDFE4AE2FDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5996FA-41A6-C449-B7F5-4B9215326876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31960" yWindow="11120" windowWidth="38140" windowHeight="24120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32340" yWindow="12160" windowWidth="38140" windowHeight="24120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA Instructions" sheetId="2" r:id="rId1"/>
@@ -486,7 +486,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="36" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -590,12 +590,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1061,7 +1055,7 @@
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="153">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -1124,12 +1118,12 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="2" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="14" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1175,13 +1169,13 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1191,135 +1185,135 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="4" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="25" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="17" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="18" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="27" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="26" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1329,37 +1323,34 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="6" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="6" borderId="13" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="29" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="28" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1377,8 +1368,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="5" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="5" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -1388,12 +1379,6 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1442,10 +1427,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="34" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1457,7 +1442,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1481,6 +1466,7 @@
     <xf numFmtId="0" fontId="9" fillId="5" borderId="24" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Hyperlink" xfId="5" builtinId="8"/>
@@ -6342,22 +6328,22 @@
       <c r="J4" s="39"/>
     </row>
     <row r="5" spans="1:10" s="37" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="126"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
+      <c r="B5" s="123"/>
+      <c r="C5" s="123"/>
+      <c r="D5" s="123"/>
+      <c r="E5" s="123"/>
       <c r="F5" s="38"/>
       <c r="H5" s="39"/>
       <c r="I5" s="40"/>
       <c r="J5" s="39"/>
     </row>
     <row r="6" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="124" t="s">
+      <c r="B6" s="121" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="124"/>
-      <c r="D6" s="124"/>
-      <c r="E6" s="124"/>
+      <c r="C6" s="121"/>
+      <c r="D6" s="121"/>
+      <c r="E6" s="121"/>
     </row>
     <row r="7" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.15">
       <c r="D7" s="43"/>
@@ -6367,62 +6353,62 @@
       <c r="A8" s="44" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="125"/>
-      <c r="C8" s="125"/>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
+      <c r="B8" s="122"/>
+      <c r="C8" s="122"/>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
     </row>
     <row r="9" spans="1:10" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="125"/>
-      <c r="C9" s="125"/>
-      <c r="D9" s="125"/>
-      <c r="E9" s="125"/>
+      <c r="B9" s="122"/>
+      <c r="C9" s="122"/>
+      <c r="D9" s="122"/>
+      <c r="E9" s="122"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A10" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="125"/>
-      <c r="C10" s="125"/>
-      <c r="D10" s="125"/>
-      <c r="E10" s="125"/>
+      <c r="B10" s="122"/>
+      <c r="C10" s="122"/>
+      <c r="D10" s="122"/>
+      <c r="E10" s="122"/>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.15">
       <c r="A11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="125"/>
-      <c r="C11" s="125"/>
-      <c r="D11" s="125"/>
-      <c r="E11" s="125"/>
+      <c r="B11" s="122"/>
+      <c r="C11" s="122"/>
+      <c r="D11" s="122"/>
+      <c r="E11" s="122"/>
     </row>
     <row r="12" spans="1:10" ht="15" x14ac:dyDescent="0.15">
       <c r="A12" s="46" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="125"/>
-      <c r="C12" s="125"/>
-      <c r="D12" s="125"/>
-      <c r="E12" s="125"/>
+      <c r="B12" s="122"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.15">
       <c r="A13" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="125"/>
-      <c r="C13" s="125"/>
-      <c r="D13" s="125"/>
-      <c r="E13" s="125"/>
+      <c r="B13" s="122"/>
+      <c r="C13" s="122"/>
+      <c r="D13" s="122"/>
+      <c r="E13" s="122"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="47"/>
-      <c r="B14" s="125"/>
-      <c r="C14" s="125"/>
-      <c r="D14" s="125"/>
-      <c r="E14" s="125"/>
+      <c r="B14" s="122"/>
+      <c r="C14" s="122"/>
+      <c r="D14" s="122"/>
+      <c r="E14" s="122"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15" s="48"/>
@@ -6451,9 +6437,9 @@
       <c r="B17" s="100" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="131"/>
-      <c r="D17" s="131"/>
-      <c r="E17" s="132"/>
+      <c r="C17" s="128"/>
+      <c r="D17" s="128"/>
+      <c r="E17" s="129"/>
       <c r="F17" s="49"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.15">
@@ -6463,9 +6449,9 @@
       <c r="B18" s="101" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="133"/>
-      <c r="D18" s="133"/>
-      <c r="E18" s="134"/>
+      <c r="C18" s="130"/>
+      <c r="D18" s="130"/>
+      <c r="E18" s="131"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" s="28" t="s">
@@ -6474,9 +6460,9 @@
       <c r="B19" s="102" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="133"/>
-      <c r="D19" s="133"/>
-      <c r="E19" s="134"/>
+      <c r="C19" s="130"/>
+      <c r="D19" s="130"/>
+      <c r="E19" s="131"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" s="28" t="s">
@@ -6485,16 +6471,16 @@
       <c r="B20" s="101" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="127"/>
-      <c r="D20" s="127"/>
-      <c r="E20" s="128"/>
+      <c r="C20" s="124"/>
+      <c r="D20" s="124"/>
+      <c r="E20" s="125"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" s="28"/>
       <c r="B21" s="90"/>
-      <c r="C21" s="127"/>
-      <c r="D21" s="127"/>
-      <c r="E21" s="128"/>
+      <c r="C21" s="124"/>
+      <c r="D21" s="124"/>
+      <c r="E21" s="125"/>
     </row>
     <row r="22" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A22" s="28" t="s">
@@ -6503,9 +6489,9 @@
       <c r="B22" s="103" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="129"/>
-      <c r="D22" s="129"/>
-      <c r="E22" s="130"/>
+      <c r="C22" s="126"/>
+      <c r="D22" s="126"/>
+      <c r="E22" s="127"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" s="28"/>
@@ -6737,7 +6723,7 @@
   <dimension ref="A1:BP120"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -7274,28 +7260,28 @@
       <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:68" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="135" t="s">
+      <c r="E2" s="132" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="136"/>
-      <c r="G2" s="136"/>
+      <c r="F2" s="133"/>
+      <c r="G2" s="133"/>
       <c r="H2" s="16"/>
       <c r="I2" s="20" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E3" s="151" t="s">
+      <c r="E3" s="148" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="152"/>
-      <c r="G3" s="152"/>
+      <c r="F3" s="149"/>
+      <c r="G3" s="149"/>
       <c r="H3" s="17"/>
       <c r="I3" s="14"/>
     </row>
     <row r="4" spans="1:68" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E4" s="119"/>
-      <c r="F4" s="147"/>
+      <c r="E4" s="118"/>
+      <c r="F4" s="144"/>
       <c r="G4" s="83" t="s">
         <v>39</v>
       </c>
@@ -7303,56 +7289,56 @@
       <c r="I4" s="14"/>
     </row>
     <row r="5" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E5" s="137" t="s">
+      <c r="E5" s="134" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="146"/>
-      <c r="G5" s="146"/>
+      <c r="F5" s="143"/>
+      <c r="G5" s="143"/>
       <c r="H5" s="17"/>
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E6" s="138" t="s">
+      <c r="E6" s="135" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="148"/>
-      <c r="G6" s="148"/>
+      <c r="F6" s="145"/>
+      <c r="G6" s="145"/>
       <c r="H6" s="17"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:68" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E7" s="121"/>
-      <c r="F7" s="149"/>
-      <c r="G7" s="120" t="s">
+      <c r="E7" s="120"/>
+      <c r="F7" s="146"/>
+      <c r="G7" s="119" t="s">
         <v>42</v>
       </c>
       <c r="H7" s="17"/>
       <c r="I7" s="18"/>
     </row>
     <row r="8" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E8" s="142" t="s">
+      <c r="E8" s="139" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="150"/>
-      <c r="G8" s="150"/>
+      <c r="F8" s="147"/>
+      <c r="G8" s="147"/>
       <c r="H8" s="17"/>
       <c r="I8" s="18"/>
     </row>
     <row r="9" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E9" s="142" t="s">
+      <c r="E9" s="139" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="150"/>
-      <c r="G9" s="150"/>
+      <c r="F9" s="147"/>
+      <c r="G9" s="147"/>
       <c r="H9" s="17"/>
       <c r="I9" s="18"/>
     </row>
     <row r="10" spans="1:68" ht="14" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E10" s="142" t="s">
+      <c r="E10" s="139" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="150"/>
-      <c r="G10" s="150"/>
+      <c r="F10" s="147"/>
+      <c r="G10" s="147"/>
       <c r="H10" s="17"/>
       <c r="I10" s="18"/>
     </row>
@@ -7361,11 +7347,11 @@
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="140" t="s">
+      <c r="E11" s="137" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="141"/>
-      <c r="G11" s="141"/>
+      <c r="F11" s="138"/>
+      <c r="G11" s="138"/>
       <c r="H11" s="13"/>
       <c r="I11" s="14"/>
     </row>
@@ -7384,14 +7370,14 @@
       <c r="L12" s="2"/>
       <c r="M12" s="2"/>
       <c r="N12" s="24"/>
-      <c r="O12" s="139" t="s">
+      <c r="O12" s="136" t="s">
         <v>47</v>
       </c>
-      <c r="P12" s="139"/>
-      <c r="Q12" s="139"/>
-      <c r="R12" s="139"/>
-      <c r="S12" s="139"/>
-      <c r="T12" s="139"/>
+      <c r="P12" s="136"/>
+      <c r="Q12" s="136"/>
+      <c r="R12" s="136"/>
+      <c r="S12" s="136"/>
+      <c r="T12" s="136"/>
     </row>
     <row r="13" spans="1:68" s="19" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72" t="s">
@@ -7447,69 +7433,69 @@
       <c r="S13" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="T13" s="111" t="s">
+      <c r="T13" s="110" t="s">
         <v>59</v>
       </c>
-      <c r="U13" s="110"/>
-      <c r="V13" s="110"/>
-      <c r="W13" s="110"/>
-      <c r="X13" s="110"/>
-      <c r="Y13" s="110"/>
-      <c r="Z13" s="110"/>
-      <c r="AA13" s="110"/>
-      <c r="AB13" s="110"/>
-      <c r="AC13" s="110"/>
-      <c r="AD13" s="110"/>
-      <c r="AE13" s="110"/>
-      <c r="AF13" s="110"/>
-      <c r="AG13" s="110"/>
-      <c r="AH13" s="110"/>
-      <c r="AI13" s="110"/>
-      <c r="AJ13" s="110"/>
-      <c r="AK13" s="110"/>
-      <c r="AL13" s="110"/>
-      <c r="AM13" s="110"/>
-      <c r="AN13" s="110"/>
-      <c r="AO13" s="110"/>
-      <c r="AP13" s="110"/>
-      <c r="AQ13" s="110"/>
-      <c r="AR13" s="110"/>
-      <c r="AS13" s="110"/>
-      <c r="AT13" s="110"/>
-      <c r="AU13" s="110"/>
-      <c r="AV13" s="110"/>
-      <c r="AW13" s="110"/>
-      <c r="AX13" s="110"/>
-      <c r="AY13" s="110"/>
-      <c r="AZ13" s="110"/>
-      <c r="BA13" s="110"/>
-      <c r="BB13" s="110"/>
-      <c r="BC13" s="110"/>
-      <c r="BD13" s="110"/>
-      <c r="BE13" s="110"/>
-      <c r="BF13" s="110"/>
-      <c r="BG13" s="110"/>
-      <c r="BH13" s="110"/>
-      <c r="BI13" s="110"/>
-      <c r="BJ13" s="110"/>
-      <c r="BK13" s="110"/>
-      <c r="BL13" s="110"/>
-      <c r="BM13" s="110"/>
-      <c r="BN13" s="110"/>
-      <c r="BO13" s="110"/>
-      <c r="BP13" s="110"/>
+      <c r="U13" s="109"/>
+      <c r="V13" s="109"/>
+      <c r="W13" s="109"/>
+      <c r="X13" s="109"/>
+      <c r="Y13" s="109"/>
+      <c r="Z13" s="109"/>
+      <c r="AA13" s="109"/>
+      <c r="AB13" s="109"/>
+      <c r="AC13" s="109"/>
+      <c r="AD13" s="109"/>
+      <c r="AE13" s="109"/>
+      <c r="AF13" s="109"/>
+      <c r="AG13" s="109"/>
+      <c r="AH13" s="109"/>
+      <c r="AI13" s="109"/>
+      <c r="AJ13" s="109"/>
+      <c r="AK13" s="109"/>
+      <c r="AL13" s="109"/>
+      <c r="AM13" s="109"/>
+      <c r="AN13" s="109"/>
+      <c r="AO13" s="109"/>
+      <c r="AP13" s="109"/>
+      <c r="AQ13" s="109"/>
+      <c r="AR13" s="109"/>
+      <c r="AS13" s="109"/>
+      <c r="AT13" s="109"/>
+      <c r="AU13" s="109"/>
+      <c r="AV13" s="109"/>
+      <c r="AW13" s="109"/>
+      <c r="AX13" s="109"/>
+      <c r="AY13" s="109"/>
+      <c r="AZ13" s="109"/>
+      <c r="BA13" s="109"/>
+      <c r="BB13" s="109"/>
+      <c r="BC13" s="109"/>
+      <c r="BD13" s="109"/>
+      <c r="BE13" s="109"/>
+      <c r="BF13" s="109"/>
+      <c r="BG13" s="109"/>
+      <c r="BH13" s="109"/>
+      <c r="BI13" s="109"/>
+      <c r="BJ13" s="109"/>
+      <c r="BK13" s="109"/>
+      <c r="BL13" s="109"/>
+      <c r="BM13" s="109"/>
+      <c r="BN13" s="109"/>
+      <c r="BO13" s="109"/>
+      <c r="BP13" s="109"/>
     </row>
     <row r="14" spans="1:68" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="109"/>
-      <c r="B14" s="122"/>
-      <c r="C14" s="122"/>
-      <c r="D14" s="122"/>
-      <c r="E14" s="108"/>
-      <c r="F14" s="108"/>
-      <c r="G14" s="77"/>
+      <c r="A14" s="150"/>
+      <c r="B14" s="150"/>
+      <c r="C14" s="150"/>
+      <c r="D14" s="150"/>
+      <c r="E14" s="150"/>
+      <c r="F14" s="150"/>
+      <c r="G14" s="150"/>
       <c r="H14" s="77"/>
       <c r="I14" s="73"/>
-      <c r="J14" s="109" t="s">
+      <c r="J14" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K14" s="78"/>
@@ -7523,17 +7509,17 @@
       <c r="S14" s="79"/>
       <c r="T14" s="80"/>
     </row>
-    <row r="15" spans="1:68" s="84" customFormat="1" ht="13" x14ac:dyDescent="0.2">
-      <c r="A15" s="109"/>
-      <c r="B15" s="122"/>
-      <c r="C15" s="122"/>
-      <c r="D15" s="122"/>
-      <c r="E15" s="108"/>
-      <c r="F15" s="108"/>
-      <c r="G15" s="76"/>
+    <row r="15" spans="1:68" s="84" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A15" s="150"/>
+      <c r="B15" s="150"/>
+      <c r="C15" s="150"/>
+      <c r="D15" s="150"/>
+      <c r="E15" s="150"/>
+      <c r="F15" s="150"/>
+      <c r="G15" s="150"/>
       <c r="H15" s="76"/>
       <c r="I15" s="73"/>
-      <c r="J15" s="109" t="s">
+      <c r="J15" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K15" s="78"/>
@@ -7548,16 +7534,16 @@
       <c r="T15" s="80"/>
     </row>
     <row r="16" spans="1:68" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="109"/>
-      <c r="B16" s="122"/>
-      <c r="C16" s="122"/>
-      <c r="D16" s="122"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
+      <c r="A16" s="150"/>
+      <c r="B16" s="150"/>
+      <c r="C16" s="150"/>
+      <c r="D16" s="150"/>
+      <c r="E16" s="150"/>
+      <c r="F16" s="150"/>
+      <c r="G16" s="150"/>
       <c r="H16" s="76"/>
       <c r="I16" s="73"/>
-      <c r="J16" s="109" t="s">
+      <c r="J16" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K16" s="78"/>
@@ -7572,16 +7558,16 @@
       <c r="T16" s="80"/>
     </row>
     <row r="17" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="122"/>
-      <c r="B17" s="122"/>
-      <c r="C17" s="122"/>
-      <c r="D17" s="122"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
+      <c r="A17" s="150"/>
+      <c r="B17" s="150"/>
+      <c r="C17" s="150"/>
+      <c r="D17" s="150"/>
+      <c r="E17" s="150"/>
+      <c r="F17" s="150"/>
+      <c r="G17" s="150"/>
       <c r="H17" s="76"/>
       <c r="I17" s="73"/>
-      <c r="J17" s="109" t="s">
+      <c r="J17" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K17" s="78"/>
@@ -7596,16 +7582,16 @@
       <c r="T17" s="80"/>
     </row>
     <row r="18" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="122"/>
-      <c r="B18" s="122"/>
-      <c r="C18" s="122"/>
-      <c r="D18" s="122"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
+      <c r="A18" s="150"/>
+      <c r="B18" s="150"/>
+      <c r="C18" s="150"/>
+      <c r="D18" s="150"/>
+      <c r="E18" s="150"/>
+      <c r="F18" s="150"/>
+      <c r="G18" s="150"/>
       <c r="H18" s="76"/>
       <c r="I18" s="73"/>
-      <c r="J18" s="109" t="s">
+      <c r="J18" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K18" s="78"/>
@@ -7620,16 +7606,16 @@
       <c r="T18" s="80"/>
     </row>
     <row r="19" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="122"/>
-      <c r="B19" s="122"/>
-      <c r="C19" s="122"/>
-      <c r="D19" s="122"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
+      <c r="A19" s="150"/>
+      <c r="B19" s="150"/>
+      <c r="C19" s="150"/>
+      <c r="D19" s="150"/>
+      <c r="E19" s="150"/>
+      <c r="F19" s="150"/>
+      <c r="G19" s="150"/>
       <c r="H19" s="76"/>
       <c r="I19" s="73"/>
-      <c r="J19" s="109" t="s">
+      <c r="J19" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K19" s="78"/>
@@ -7644,16 +7630,16 @@
       <c r="T19" s="80"/>
     </row>
     <row r="20" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="122"/>
-      <c r="B20" s="122"/>
-      <c r="C20" s="122"/>
-      <c r="D20" s="122"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
+      <c r="A20" s="150"/>
+      <c r="B20" s="150"/>
+      <c r="C20" s="150"/>
+      <c r="D20" s="150"/>
+      <c r="E20" s="150"/>
+      <c r="F20" s="150"/>
+      <c r="G20" s="150"/>
       <c r="H20" s="76"/>
       <c r="I20" s="73"/>
-      <c r="J20" s="109" t="s">
+      <c r="J20" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K20" s="78"/>
@@ -7668,16 +7654,16 @@
       <c r="T20" s="80"/>
     </row>
     <row r="21" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="123"/>
-      <c r="B21" s="123"/>
-      <c r="C21" s="123"/>
-      <c r="D21" s="123"/>
-      <c r="E21" s="73"/>
-      <c r="F21" s="73"/>
-      <c r="G21" s="73"/>
+      <c r="A21" s="150"/>
+      <c r="B21" s="150"/>
+      <c r="C21" s="150"/>
+      <c r="D21" s="150"/>
+      <c r="E21" s="150"/>
+      <c r="F21" s="150"/>
+      <c r="G21" s="150"/>
       <c r="H21" s="73"/>
       <c r="I21" s="81"/>
-      <c r="J21" s="109" t="s">
+      <c r="J21" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K21" s="79"/>
@@ -7692,16 +7678,16 @@
       <c r="T21" s="73"/>
     </row>
     <row r="22" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="123"/>
-      <c r="B22" s="123"/>
-      <c r="C22" s="123"/>
-      <c r="D22" s="123"/>
-      <c r="E22" s="73"/>
-      <c r="F22" s="73"/>
-      <c r="G22" s="73"/>
+      <c r="A22" s="150"/>
+      <c r="B22" s="150"/>
+      <c r="C22" s="150"/>
+      <c r="D22" s="150"/>
+      <c r="E22" s="150"/>
+      <c r="F22" s="150"/>
+      <c r="G22" s="150"/>
       <c r="H22" s="73"/>
       <c r="I22" s="73"/>
-      <c r="J22" s="109" t="s">
+      <c r="J22" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K22" s="73"/>
@@ -7716,16 +7702,16 @@
       <c r="T22" s="73"/>
     </row>
     <row r="23" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="123"/>
-      <c r="B23" s="123"/>
-      <c r="C23" s="123"/>
-      <c r="D23" s="123"/>
-      <c r="E23" s="73"/>
-      <c r="F23" s="73"/>
-      <c r="G23" s="73"/>
+      <c r="A23" s="150"/>
+      <c r="B23" s="150"/>
+      <c r="C23" s="150"/>
+      <c r="D23" s="150"/>
+      <c r="E23" s="150"/>
+      <c r="F23" s="150"/>
+      <c r="G23" s="150"/>
       <c r="H23" s="73"/>
       <c r="I23" s="73"/>
-      <c r="J23" s="109" t="s">
+      <c r="J23" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K23" s="73"/>
@@ -7740,16 +7726,16 @@
       <c r="T23" s="73"/>
     </row>
     <row r="24" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="123"/>
-      <c r="B24" s="123"/>
-      <c r="C24" s="123"/>
-      <c r="D24" s="123"/>
-      <c r="E24" s="73"/>
-      <c r="F24" s="73"/>
-      <c r="G24" s="73"/>
+      <c r="A24" s="150"/>
+      <c r="B24" s="150"/>
+      <c r="C24" s="150"/>
+      <c r="D24" s="150"/>
+      <c r="E24" s="150"/>
+      <c r="F24" s="150"/>
+      <c r="G24" s="150"/>
       <c r="H24" s="73"/>
       <c r="I24" s="73"/>
-      <c r="J24" s="109" t="s">
+      <c r="J24" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K24" s="73"/>
@@ -7764,16 +7750,16 @@
       <c r="T24" s="73"/>
     </row>
     <row r="25" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="123"/>
-      <c r="B25" s="123"/>
-      <c r="C25" s="123"/>
-      <c r="D25" s="123"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="73"/>
-      <c r="G25" s="73"/>
+      <c r="A25" s="150"/>
+      <c r="B25" s="150"/>
+      <c r="C25" s="150"/>
+      <c r="D25" s="150"/>
+      <c r="E25" s="150"/>
+      <c r="F25" s="150"/>
+      <c r="G25" s="150"/>
       <c r="H25" s="73"/>
       <c r="I25" s="73"/>
-      <c r="J25" s="109" t="s">
+      <c r="J25" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K25" s="73"/>
@@ -7788,16 +7774,16 @@
       <c r="T25" s="73"/>
     </row>
     <row r="26" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="123"/>
-      <c r="B26" s="123"/>
-      <c r="C26" s="123"/>
-      <c r="D26" s="123"/>
-      <c r="E26" s="73"/>
-      <c r="F26" s="73"/>
-      <c r="G26" s="73"/>
+      <c r="A26" s="150"/>
+      <c r="B26" s="150"/>
+      <c r="C26" s="150"/>
+      <c r="D26" s="150"/>
+      <c r="E26" s="150"/>
+      <c r="F26" s="150"/>
+      <c r="G26" s="150"/>
       <c r="H26" s="73"/>
       <c r="I26" s="73"/>
-      <c r="J26" s="109" t="s">
+      <c r="J26" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K26" s="73"/>
@@ -7812,16 +7798,16 @@
       <c r="T26" s="73"/>
     </row>
     <row r="27" spans="1:20" s="84" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="123"/>
-      <c r="B27" s="123"/>
-      <c r="C27" s="123"/>
-      <c r="D27" s="123"/>
-      <c r="E27" s="73"/>
-      <c r="F27" s="73"/>
-      <c r="G27" s="73"/>
+      <c r="A27" s="150"/>
+      <c r="B27" s="150"/>
+      <c r="C27" s="150"/>
+      <c r="D27" s="150"/>
+      <c r="E27" s="150"/>
+      <c r="F27" s="150"/>
+      <c r="G27" s="150"/>
       <c r="H27" s="73"/>
       <c r="I27" s="73"/>
-      <c r="J27" s="109" t="s">
+      <c r="J27" s="108" t="s">
         <v>60</v>
       </c>
       <c r="K27" s="73"/>
@@ -9342,10 +9328,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="123" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="143" t="s">
+      <c r="A1" s="140" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="144"/>
+      <c r="B1" s="141"/>
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
       <c r="E1" s="43"/>
@@ -9392,12 +9378,12 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A8" s="112" t="s">
+      <c r="A8" s="111" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="112" t="s">
         <v>72</v>
       </c>
     </row>
@@ -9424,237 +9410,237 @@
     <col min="3" max="16384" width="9.1640625" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="118" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="145" t="s">
+    <row r="1" spans="1:3" s="117" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="142" t="s">
         <v>73</v>
       </c>
-      <c r="B1" s="145"/>
+      <c r="B1" s="142"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A2" s="114"/>
-      <c r="B2" s="114"/>
-      <c r="C2" s="114"/>
+      <c r="A2" s="113"/>
+      <c r="B2" s="113"/>
+      <c r="C2" s="113"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A3" s="115" t="s">
+      <c r="A3" s="114" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="115" t="s">
+      <c r="B3" s="114" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="114"/>
+      <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
-      <c r="A4" s="116" t="s">
+      <c r="A4" s="115" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="114" t="s">
+      <c r="B4" s="113" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="114"/>
+      <c r="C4" s="113"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A5" s="116" t="s">
+      <c r="A5" s="115" t="s">
         <v>78</v>
       </c>
-      <c r="B5" s="117" t="s">
+      <c r="B5" s="116" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="114"/>
+      <c r="C5" s="113"/>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="115" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="117" t="s">
+      <c r="B6" s="116" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="114"/>
+      <c r="C6" s="113"/>
     </row>
     <row r="7" spans="1:3" ht="56.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="116"/>
-      <c r="B7" s="114"/>
-      <c r="C7" s="114"/>
+      <c r="A7" s="115"/>
+      <c r="B7" s="113"/>
+      <c r="C7" s="113"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A8" s="116"/>
-      <c r="B8" s="114"/>
-      <c r="C8" s="114"/>
+      <c r="A8" s="115"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="113"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A9" s="114"/>
-      <c r="B9" s="114"/>
-      <c r="C9" s="114"/>
+      <c r="A9" s="113"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="113"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A10" s="114"/>
-      <c r="B10" s="114"/>
-      <c r="C10" s="114"/>
+      <c r="A10" s="113"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="113"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A11" s="114"/>
-      <c r="B11" s="114"/>
-      <c r="C11" s="114"/>
+      <c r="A11" s="113"/>
+      <c r="B11" s="113"/>
+      <c r="C11" s="113"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A12" s="114"/>
-      <c r="B12" s="114"/>
-      <c r="C12" s="114"/>
+      <c r="A12" s="113"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="113"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A13" s="114"/>
-      <c r="B13" s="114"/>
-      <c r="C13" s="114"/>
+      <c r="A13" s="113"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="113"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A14" s="114"/>
-      <c r="B14" s="114"/>
-      <c r="C14" s="114"/>
+      <c r="A14" s="113"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="113"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A15" s="114"/>
-      <c r="B15" s="114"/>
-      <c r="C15" s="114"/>
+      <c r="A15" s="113"/>
+      <c r="B15" s="113"/>
+      <c r="C15" s="113"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A16" s="114"/>
-      <c r="B16" s="114"/>
-      <c r="C16" s="114"/>
+      <c r="A16" s="113"/>
+      <c r="B16" s="113"/>
+      <c r="C16" s="113"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A17" s="114"/>
-      <c r="B17" s="114"/>
-      <c r="C17" s="114"/>
+      <c r="A17" s="113"/>
+      <c r="B17" s="113"/>
+      <c r="C17" s="113"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A18" s="114"/>
-      <c r="B18" s="114"/>
-      <c r="C18" s="114"/>
+      <c r="A18" s="113"/>
+      <c r="B18" s="113"/>
+      <c r="C18" s="113"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A19" s="114"/>
-      <c r="B19" s="114"/>
-      <c r="C19" s="114"/>
+      <c r="A19" s="113"/>
+      <c r="B19" s="113"/>
+      <c r="C19" s="113"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A20" s="114"/>
-      <c r="B20" s="114"/>
-      <c r="C20" s="114"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
+      <c r="C20" s="113"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A21" s="114"/>
-      <c r="B21" s="114"/>
-      <c r="C21" s="114"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
+      <c r="C21" s="113"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A22" s="114"/>
-      <c r="B22" s="114"/>
-      <c r="C22" s="114"/>
+      <c r="A22" s="113"/>
+      <c r="B22" s="113"/>
+      <c r="C22" s="113"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A23" s="114"/>
-      <c r="B23" s="114"/>
-      <c r="C23" s="114"/>
+      <c r="A23" s="113"/>
+      <c r="B23" s="113"/>
+      <c r="C23" s="113"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A24" s="114"/>
-      <c r="B24" s="114"/>
-      <c r="C24" s="114"/>
+      <c r="A24" s="113"/>
+      <c r="B24" s="113"/>
+      <c r="C24" s="113"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A25" s="114"/>
-      <c r="B25" s="114"/>
-      <c r="C25" s="114"/>
+      <c r="A25" s="113"/>
+      <c r="B25" s="113"/>
+      <c r="C25" s="113"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A26" s="114"/>
-      <c r="B26" s="114"/>
-      <c r="C26" s="114"/>
+      <c r="A26" s="113"/>
+      <c r="B26" s="113"/>
+      <c r="C26" s="113"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A27" s="114"/>
-      <c r="B27" s="114"/>
-      <c r="C27" s="114"/>
+      <c r="A27" s="113"/>
+      <c r="B27" s="113"/>
+      <c r="C27" s="113"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A28" s="114"/>
-      <c r="B28" s="114"/>
-      <c r="C28" s="114"/>
+      <c r="A28" s="113"/>
+      <c r="B28" s="113"/>
+      <c r="C28" s="113"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A29" s="114"/>
-      <c r="B29" s="114"/>
-      <c r="C29" s="114"/>
+      <c r="A29" s="113"/>
+      <c r="B29" s="113"/>
+      <c r="C29" s="113"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A30" s="114"/>
-      <c r="B30" s="114"/>
-      <c r="C30" s="114"/>
+      <c r="A30" s="113"/>
+      <c r="B30" s="113"/>
+      <c r="C30" s="113"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A31" s="114"/>
-      <c r="B31" s="114"/>
-      <c r="C31" s="114"/>
+      <c r="A31" s="113"/>
+      <c r="B31" s="113"/>
+      <c r="C31" s="113"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A32" s="114"/>
-      <c r="B32" s="114"/>
-      <c r="C32" s="114"/>
+      <c r="A32" s="113"/>
+      <c r="B32" s="113"/>
+      <c r="C32" s="113"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A33" s="114"/>
-      <c r="B33" s="114"/>
-      <c r="C33" s="114"/>
+      <c r="A33" s="113"/>
+      <c r="B33" s="113"/>
+      <c r="C33" s="113"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A34" s="114"/>
-      <c r="B34" s="114"/>
-      <c r="C34" s="114"/>
+      <c r="A34" s="113"/>
+      <c r="B34" s="113"/>
+      <c r="C34" s="113"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A35" s="114"/>
-      <c r="B35" s="114"/>
-      <c r="C35" s="114"/>
+      <c r="A35" s="113"/>
+      <c r="B35" s="113"/>
+      <c r="C35" s="113"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A36" s="114"/>
-      <c r="B36" s="114"/>
-      <c r="C36" s="114"/>
+      <c r="A36" s="113"/>
+      <c r="B36" s="113"/>
+      <c r="C36" s="113"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A37" s="114"/>
-      <c r="B37" s="114"/>
-      <c r="C37" s="114"/>
+      <c r="A37" s="113"/>
+      <c r="B37" s="113"/>
+      <c r="C37" s="113"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A38" s="114"/>
-      <c r="B38" s="114"/>
-      <c r="C38" s="114"/>
+      <c r="A38" s="113"/>
+      <c r="B38" s="113"/>
+      <c r="C38" s="113"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A39" s="114"/>
-      <c r="B39" s="114"/>
-      <c r="C39" s="114"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
+      <c r="C39" s="113"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A40" s="114"/>
-      <c r="B40" s="114"/>
-      <c r="C40" s="114"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
+      <c r="C40" s="113"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A41" s="114"/>
-      <c r="B41" s="114"/>
-      <c r="C41" s="114"/>
+      <c r="A41" s="113"/>
+      <c r="B41" s="113"/>
+      <c r="C41" s="113"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A42" s="114"/>
-      <c r="B42" s="114"/>
-      <c r="C42" s="114"/>
+      <c r="A42" s="113"/>
+      <c r="B42" s="113"/>
+      <c r="C42" s="113"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.15">
-      <c r="A43" s="114"/>
-      <c r="B43" s="114"/>
-      <c r="C43" s="114"/>
+      <c r="A43" s="113"/>
+      <c r="B43" s="113"/>
+      <c r="C43" s="113"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
updated section names and column sizes
</commit_message>
<xml_diff>
--- a/inst/extdata/QA_Template_Coded_Analysis.xlsx
+++ b/inst/extdata/QA_Template_Coded_Analysis.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzadra41/Documents/R Projects/integral-private/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3098E81F-C38F-A14B-8B6F-758FE87AFC72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5168741-7909-7A49-8634-BEA8056B523F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34340" yWindow="16620" windowWidth="38140" windowHeight="24120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="34340" yWindow="16580" windowWidth="38140" windowHeight="24120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA Instructions" sheetId="2" r:id="rId1"/>
-    <sheet name="Code_Review_Template" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="Code_Review_Template" sheetId="3" r:id="rId2"/>
     <sheet name="QA Tags" sheetId="4" r:id="rId3"/>
     <sheet name="Resources" sheetId="6" r:id="rId4"/>
   </sheets>
@@ -239,9 +239,6 @@
       </rPr>
       <t>)</t>
     </r>
-  </si>
-  <si>
-    <t>Section</t>
   </si>
   <si>
     <t>Review Instructions</t>
@@ -470,13 +467,20 @@
     <t>Line Number (Approximate)</t>
   </si>
   <si>
-    <t>Subsection</t>
+    <t>Section
+Level 1</t>
   </si>
   <si>
-    <t>Level 3</t>
+    <t>Section
+Level 2</t>
   </si>
   <si>
-    <t>Level 4</t>
+    <t>Section
+Level 3</t>
+  </si>
+  <si>
+    <t>Section
+Level 4</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1859,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -1922,7 +1926,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>11289</xdr:rowOff>
         </xdr:to>
@@ -1989,7 +1993,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -2056,7 +2060,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2123,7 +2127,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2190,7 +2194,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:to>
@@ -2257,7 +2261,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:to>
@@ -2324,7 +2328,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -2391,7 +2395,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -2458,7 +2462,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -2525,7 +2529,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -2592,7 +2596,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>203200</xdr:rowOff>
         </xdr:to>
@@ -2659,7 +2663,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -2726,7 +2730,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -2793,7 +2797,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2860,7 +2864,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2927,7 +2931,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -2994,7 +2998,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:to>
@@ -3061,7 +3065,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:to>
@@ -3128,7 +3132,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>177800</xdr:rowOff>
         </xdr:to>
@@ -3195,7 +3199,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -3262,7 +3266,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -3329,7 +3333,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -3396,7 +3400,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -3463,7 +3467,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -3530,7 +3534,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -3597,7 +3601,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>203200</xdr:rowOff>
         </xdr:to>
@@ -3664,7 +3668,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>203200</xdr:rowOff>
         </xdr:to>
@@ -3731,7 +3735,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3798,7 +3802,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3865,7 +3869,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3932,7 +3936,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -3999,7 +4003,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4066,7 +4070,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4133,7 +4137,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4200,7 +4204,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4267,7 +4271,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4334,7 +4338,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4401,7 +4405,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -4468,7 +4472,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -4535,7 +4539,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -4602,7 +4606,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -4669,7 +4673,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>25401</xdr:rowOff>
         </xdr:to>
@@ -4736,7 +4740,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -4803,7 +4807,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -4870,7 +4874,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -4937,7 +4941,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5004,7 +5008,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5071,7 +5075,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5138,7 +5142,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5205,7 +5209,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5272,7 +5276,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5339,7 +5343,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5406,7 +5410,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5473,7 +5477,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5540,7 +5544,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5607,7 +5611,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5674,7 +5678,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -5741,7 +5745,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5808,7 +5812,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>609601</xdr:colOff>
+          <xdr:colOff>609600</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>25400</xdr:rowOff>
         </xdr:to>
@@ -5875,7 +5879,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>8</xdr:col>
-          <xdr:colOff>114301</xdr:colOff>
+          <xdr:colOff>114300</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>63500</xdr:rowOff>
         </xdr:to>
@@ -6722,14 +6726,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BP120"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="4" width="18.33203125" style="15" customWidth="1"/>
-    <col min="5" max="6" width="20.6640625" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" style="15" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="15" customWidth="1"/>
     <col min="7" max="7" width="42.5" style="15" customWidth="1"/>
     <col min="8" max="8" width="3" style="15" customWidth="1"/>
     <col min="9" max="9" width="44" style="15" customWidth="1"/>
@@ -7381,7 +7386,7 @@
     </row>
     <row r="13" spans="1:68" s="19" customFormat="1" ht="54.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="72" t="s">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="B13" s="72" t="s">
         <v>84</v>
@@ -7393,48 +7398,48 @@
         <v>86</v>
       </c>
       <c r="E13" s="72" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F13" s="72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G13" s="98" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="H13" s="72"/>
       <c r="I13" s="72" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="99" t="s">
         <v>50</v>
       </c>
-      <c r="J13" s="99" t="s">
+      <c r="K13" s="72" t="s">
         <v>51</v>
       </c>
-      <c r="K13" s="72" t="s">
+      <c r="L13" s="72" t="s">
         <v>52</v>
       </c>
-      <c r="L13" s="72" t="s">
+      <c r="M13" s="72" t="s">
         <v>53</v>
-      </c>
-      <c r="M13" s="72" t="s">
-        <v>54</v>
       </c>
       <c r="N13" s="25"/>
       <c r="O13" s="72" t="s">
+        <v>54</v>
+      </c>
+      <c r="P13" s="72" t="s">
         <v>55</v>
       </c>
-      <c r="P13" s="72" t="s">
+      <c r="Q13" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="Q13" s="72" t="s">
+      <c r="R13" s="72" t="s">
         <v>57</v>
       </c>
-      <c r="R13" s="72" t="s">
+      <c r="S13" s="72" t="s">
+        <v>52</v>
+      </c>
+      <c r="T13" s="110" t="s">
         <v>58</v>
-      </c>
-      <c r="S13" s="72" t="s">
-        <v>53</v>
-      </c>
-      <c r="T13" s="110" t="s">
-        <v>59</v>
       </c>
       <c r="U13" s="109"/>
       <c r="V13" s="109"/>
@@ -7496,7 +7501,7 @@
       <c r="H14" s="77"/>
       <c r="I14" s="73"/>
       <c r="J14" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K14" s="78"/>
       <c r="L14" s="79"/>
@@ -7520,7 +7525,7 @@
       <c r="H15" s="76"/>
       <c r="I15" s="73"/>
       <c r="J15" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K15" s="78"/>
       <c r="L15" s="79"/>
@@ -7544,7 +7549,7 @@
       <c r="H16" s="76"/>
       <c r="I16" s="73"/>
       <c r="J16" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K16" s="78"/>
       <c r="L16" s="79"/>
@@ -7568,7 +7573,7 @@
       <c r="H17" s="76"/>
       <c r="I17" s="73"/>
       <c r="J17" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K17" s="78"/>
       <c r="L17" s="79"/>
@@ -7592,7 +7597,7 @@
       <c r="H18" s="76"/>
       <c r="I18" s="73"/>
       <c r="J18" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K18" s="78"/>
       <c r="L18" s="79"/>
@@ -7616,7 +7621,7 @@
       <c r="H19" s="76"/>
       <c r="I19" s="73"/>
       <c r="J19" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K19" s="78"/>
       <c r="L19" s="79"/>
@@ -7640,7 +7645,7 @@
       <c r="H20" s="76"/>
       <c r="I20" s="73"/>
       <c r="J20" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K20" s="78"/>
       <c r="L20" s="79"/>
@@ -7664,7 +7669,7 @@
       <c r="H21" s="73"/>
       <c r="I21" s="81"/>
       <c r="J21" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K21" s="79"/>
       <c r="L21" s="80"/>
@@ -7688,7 +7693,7 @@
       <c r="H22" s="73"/>
       <c r="I22" s="73"/>
       <c r="J22" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K22" s="73"/>
       <c r="L22" s="73"/>
@@ -7712,7 +7717,7 @@
       <c r="H23" s="73"/>
       <c r="I23" s="73"/>
       <c r="J23" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K23" s="73"/>
       <c r="L23" s="73"/>
@@ -7736,7 +7741,7 @@
       <c r="H24" s="73"/>
       <c r="I24" s="73"/>
       <c r="J24" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K24" s="73"/>
       <c r="L24" s="73"/>
@@ -7760,7 +7765,7 @@
       <c r="H25" s="73"/>
       <c r="I25" s="73"/>
       <c r="J25" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K25" s="73"/>
       <c r="L25" s="73"/>
@@ -7784,7 +7789,7 @@
       <c r="H26" s="73"/>
       <c r="I26" s="73"/>
       <c r="J26" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K26" s="73"/>
       <c r="L26" s="73"/>
@@ -7808,7 +7813,7 @@
       <c r="H27" s="73"/>
       <c r="I27" s="73"/>
       <c r="J27" s="108" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K27" s="73"/>
       <c r="L27" s="73"/>
@@ -9316,7 +9321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="AJ1" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -9329,7 +9334,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="123" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="140" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B1" s="141"/>
       <c r="C1" s="43"/>
@@ -9339,7 +9344,7 @@
     </row>
     <row r="2" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="10" t="s">
         <v>15</v>
@@ -9347,44 +9352,44 @@
     </row>
     <row r="3" spans="1:6" ht="57" thickTop="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="56" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>67</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A6" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" s="111" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" s="112" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -9412,7 +9417,7 @@
   <sheetData>
     <row r="1" spans="1:3" s="117" customFormat="1" ht="55.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="142" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B1" s="142"/>
     </row>
@@ -9423,37 +9428,37 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" s="114" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="114" t="s">
         <v>74</v>
-      </c>
-      <c r="B3" s="114" t="s">
-        <v>75</v>
       </c>
       <c r="C3" s="113"/>
     </row>
     <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.15">
       <c r="A4" s="115" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" s="113" t="s">
         <v>76</v>
-      </c>
-      <c r="B4" s="113" t="s">
-        <v>77</v>
       </c>
       <c r="C4" s="113"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" s="115" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5" s="116" t="s">
         <v>78</v>
-      </c>
-      <c r="B5" s="116" t="s">
-        <v>79</v>
       </c>
       <c r="C5" s="113"/>
     </row>
     <row r="6" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="115" t="s">
+        <v>79</v>
+      </c>
+      <c r="B6" s="116" t="s">
         <v>80</v>
-      </c>
-      <c r="B6" s="116" t="s">
-        <v>81</v>
       </c>
       <c r="C6" s="113"/>
     </row>

</xml_diff>

<commit_message>
removed tags column and hid tags sheet.
</commit_message>
<xml_diff>
--- a/inst/extdata/QA_Template_Coded_Analysis.xlsx
+++ b/inst/extdata/QA_Template_Coded_Analysis.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzadra41/Documents/R Projects/integral-private/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4167F9AF-F7CA-9A4C-86A3-7E5D675D2F54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9572DE83-A1BF-E24E-B4C7-5A05A9ACFAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18860" yWindow="500" windowWidth="38780" windowHeight="22540" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18860" yWindow="500" windowWidth="38780" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QA Instructions" sheetId="1" r:id="rId1"/>
     <sheet name="Code_Review_Template" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="QA Tags" sheetId="3" r:id="rId3"/>
+    <sheet name="QA Tags" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="sections">Code_Review_Template!$A$14:$D$39</definedName>
-    <definedName name="tags">Code_Review_Template!$J$14:$J$40</definedName>
+    <definedName name="tags">Code_Review_Template!#REF!</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>Privileged and Confidential</t>
   </si>
@@ -282,9 +282,6 @@
     <t xml:space="preserve">Findings </t>
   </si>
   <si>
-    <t xml:space="preserve">Tag for Findings </t>
-  </si>
-  <si>
     <t>QA completed by</t>
   </si>
   <si>
@@ -309,9 +306,6 @@
   <si>
     <t>Author Response 
 (Initials, rationale, or confirmation that issue was corrected in the code)</t>
-  </si>
-  <si>
-    <t>#tag</t>
   </si>
   <si>
     <r>
@@ -467,7 +461,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
   </numFmts>
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="31" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -651,15 +645,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -668,13 +653,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FFC00000"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -1016,13 +994,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="129">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1252,9 +1230,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="2" borderId="4" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1264,20 +1239,17 @@
     <xf numFmtId="0" fontId="15" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="4" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1301,6 +1273,31 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="26" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1345,34 +1342,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="8" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="27" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1504,7 +1473,43 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp19.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp2.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp20.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp21.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp22.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp23.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp24.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp25.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp26.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp27.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -1652,7 +1657,7 @@
                   <a14:compatExt spid="_x0000_s1001"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6A924C2-E83D-48F5-3778-BF697982E23B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000E9030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1729,7 +1734,7 @@
                   <a14:compatExt spid="_x0000_s1002"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{453C14A9-DBB9-C744-7293-1422B85FB85D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000EA030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1806,7 +1811,7 @@
                   <a14:compatExt spid="_x0000_s1003"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E8B8361-73C7-ABFE-4ADF-7C789B0A3783}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000EB030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1883,7 +1888,7 @@
                   <a14:compatExt spid="_x0000_s1004"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C9E92BE-23CA-89C6-309E-72F95D50F5EF}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000EC030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1960,7 +1965,7 @@
                   <a14:compatExt spid="_x0000_s1005"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F3C07A1-F1F7-BEC0-BA95-AFA2961E7CF2}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000ED030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2037,7 +2042,7 @@
                   <a14:compatExt spid="_x0000_s1006"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60344DFA-04BC-4AAE-54A3-1E5FE2E9D4D1}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000EE030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2114,7 +2119,7 @@
                   <a14:compatExt spid="_x0000_s1007"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFD0FE93-FAFB-2A1E-44FD-B673A7CCB3E4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000EF030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2191,7 +2196,7 @@
                   <a14:compatExt spid="_x0000_s1008"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E8C9944A-500A-375B-5761-A88F6CE84525}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000F0030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2268,7 +2273,7 @@
                   <a14:compatExt spid="_x0000_s1009"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2041C48B-6F3D-5745-22B7-D98CECEB03D8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-0000F1030000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2345,7 +2350,7 @@
                   <a14:compatExt spid="_x0000_s2057"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCD5F9C4-FE63-9C09-CF37-222407886189}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000009080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2412,7 +2417,7 @@
                   <a14:compatExt spid="_x0000_s2056"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCCBDC24-1BED-D0DF-080C-BE83BBC5CCC7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000008080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2479,7 +2484,7 @@
                   <a14:compatExt spid="_x0000_s2055"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1DD8DEA-26B3-0D07-65B6-2A6AE2B9849D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000007080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2546,7 +2551,7 @@
                   <a14:compatExt spid="_x0000_s2054"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98314B6A-C42D-F1F9-5490-B3763E2FEBDB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000006080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2613,7 +2618,7 @@
                   <a14:compatExt spid="_x0000_s2053"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA54291C-CCB2-3E77-4B49-33BF9338418B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000005080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2680,7 +2685,7 @@
                   <a14:compatExt spid="_x0000_s2052"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A28CAF8F-0225-D38F-5BE1-29647977015E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000004080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2747,7 +2752,7 @@
                   <a14:compatExt spid="_x0000_s2051"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{718235C0-EC72-C09B-BD5D-FD2612174555}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2814,7 +2819,7 @@
                   <a14:compatExt spid="_x0000_s2050"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D9134044-CB67-66A4-DC75-3415CBA89820}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2881,7 +2886,610 @@
                   <a14:compatExt spid="_x0000_s2049"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E93D5197-C0B5-0282-D734-E0430DAA85D7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2066" name="Check Box 18" descr="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2066"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000012080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2065" name="Check Box 17" descr="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2065"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000011080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2064" name="Check Box 16" descr="Check Box 39" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2064"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000010080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2063" name="Check Box 15" descr="Check Box 44" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2063"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000F080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2062" name="Check Box 14" descr="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2062"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000E080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2061" name="Check Box 13" descr="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2061"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000D080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2060" name="Check Box 12" descr="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2060"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000C080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2059" name="Check Box 11" descr="Check Box 62" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2059"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000B080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2058" name="Check Box 10" descr="Check Box 64" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2058"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3231,7 +3839,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ54"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -3299,22 +3907,22 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" s="7" customFormat="1" ht="14" x14ac:dyDescent="0.15">
-      <c r="B5" s="107"/>
-      <c r="C5" s="107"/>
-      <c r="D5" s="107"/>
-      <c r="E5" s="107"/>
+      <c r="B5" s="114"/>
+      <c r="C5" s="114"/>
+      <c r="D5" s="114"/>
+      <c r="E5" s="114"/>
       <c r="F5" s="8"/>
       <c r="H5" s="9"/>
       <c r="I5" s="10"/>
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="B6" s="108" t="s">
+      <c r="B6" s="115" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="108"/>
-      <c r="D6" s="108"/>
-      <c r="E6" s="108"/>
+      <c r="C6" s="115"/>
+      <c r="D6" s="115"/>
+      <c r="E6" s="115"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="D7" s="17"/>
@@ -3324,62 +3932,62 @@
       <c r="A8" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="109"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="109"/>
-      <c r="E8" s="109"/>
+      <c r="B8" s="116"/>
+      <c r="C8" s="116"/>
+      <c r="D8" s="116"/>
+      <c r="E8" s="116"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="109"/>
-      <c r="C9" s="109"/>
-      <c r="D9" s="109"/>
-      <c r="E9" s="109"/>
+      <c r="B9" s="116"/>
+      <c r="C9" s="116"/>
+      <c r="D9" s="116"/>
+      <c r="E9" s="116"/>
     </row>
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="109"/>
-      <c r="C10" s="109"/>
-      <c r="D10" s="109"/>
-      <c r="E10" s="109"/>
+      <c r="B10" s="116"/>
+      <c r="C10" s="116"/>
+      <c r="D10" s="116"/>
+      <c r="E10" s="116"/>
     </row>
     <row r="11" spans="1:10" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="109"/>
-      <c r="C11" s="109"/>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="116"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="109"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="109"/>
-      <c r="E12" s="109"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="116"/>
     </row>
     <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.2">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="109"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="109"/>
-      <c r="E13" s="109"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="116"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="21"/>
-      <c r="B14" s="109"/>
-      <c r="C14" s="109"/>
-      <c r="D14" s="109"/>
-      <c r="E14" s="109"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="116"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="22"/>
@@ -3408,9 +4016,9 @@
       <c r="B17" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="110"/>
-      <c r="D17" s="110"/>
-      <c r="E17" s="110"/>
+      <c r="C17" s="117"/>
+      <c r="D17" s="117"/>
+      <c r="E17" s="117"/>
       <c r="F17" s="28"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -3420,9 +4028,9 @@
       <c r="B18" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="C18" s="104"/>
-      <c r="D18" s="104"/>
-      <c r="E18" s="104"/>
+      <c r="C18" s="111"/>
+      <c r="D18" s="111"/>
+      <c r="E18" s="111"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="23" t="s">
@@ -3431,9 +4039,9 @@
       <c r="B19" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="104"/>
-      <c r="D19" s="104"/>
-      <c r="E19" s="104"/>
+      <c r="C19" s="111"/>
+      <c r="D19" s="111"/>
+      <c r="E19" s="111"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="23" t="s">
@@ -3442,16 +4050,16 @@
       <c r="B20" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="C20" s="105"/>
-      <c r="D20" s="105"/>
-      <c r="E20" s="105"/>
+      <c r="C20" s="112"/>
+      <c r="D20" s="112"/>
+      <c r="E20" s="112"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="23"/>
       <c r="B21" s="32"/>
-      <c r="C21" s="105"/>
-      <c r="D21" s="105"/>
-      <c r="E21" s="105"/>
+      <c r="C21" s="112"/>
+      <c r="D21" s="112"/>
+      <c r="E21" s="112"/>
     </row>
     <row r="22" spans="1:6" ht="42" x14ac:dyDescent="0.2">
       <c r="A22" s="23" t="s">
@@ -3460,9 +4068,9 @@
       <c r="B22" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="106"/>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
+      <c r="C22" s="113"/>
+      <c r="D22" s="113"/>
+      <c r="E22" s="113"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="23"/>
@@ -3691,10 +4299,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:T107"/>
+  <dimension ref="A1:S107"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3705,20 +4313,19 @@
     <col min="7" max="7" width="42.5" style="1" customWidth="1"/>
     <col min="8" max="8" width="3" style="1" customWidth="1"/>
     <col min="9" max="9" width="44" style="1" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" style="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.33203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="27.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="2.5" style="69" customWidth="1"/>
-    <col min="15" max="15" width="19.5" style="1" customWidth="1"/>
-    <col min="16" max="16" width="18.83203125" style="1" customWidth="1"/>
-    <col min="17" max="17" width="14" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.33203125" style="1" customWidth="1"/>
-    <col min="19" max="19" width="8" style="1" customWidth="1"/>
-    <col min="20" max="20" width="28.1640625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" style="1" customWidth="1"/>
+    <col min="12" max="12" width="27.6640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="2.5" style="69" customWidth="1"/>
+    <col min="14" max="14" width="19.5" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="14" style="1" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" style="1" customWidth="1"/>
+    <col min="18" max="18" width="8" style="1" customWidth="1"/>
+    <col min="19" max="19" width="28.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="70" t="s">
         <v>0</v>
       </c>
@@ -3726,27 +4333,27 @@
       <c r="C1" s="70"/>
       <c r="D1" s="70"/>
     </row>
-    <row r="2" spans="1:20" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E2" s="114" t="s">
+    <row r="2" spans="1:19" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E2" s="121" t="s">
         <v>36</v>
       </c>
-      <c r="F2" s="114"/>
-      <c r="G2" s="114"/>
+      <c r="F2" s="121"/>
+      <c r="G2" s="121"/>
       <c r="H2" s="71"/>
       <c r="I2" s="72" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E3" s="115" t="s">
+    <row r="3" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="F3" s="115"/>
-      <c r="G3" s="115"/>
+      <c r="F3" s="122"/>
+      <c r="G3" s="122"/>
       <c r="H3" s="73"/>
       <c r="I3" s="74"/>
     </row>
-    <row r="4" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E4" s="75"/>
       <c r="F4" s="76"/>
       <c r="G4" s="77" t="s">
@@ -3755,25 +4362,25 @@
       <c r="H4" s="73"/>
       <c r="I4" s="74"/>
     </row>
-    <row r="5" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E5" s="116" t="s">
+    <row r="5" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="123" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="116"/>
-      <c r="G5" s="116"/>
+      <c r="F5" s="123"/>
+      <c r="G5" s="123"/>
       <c r="H5" s="73"/>
       <c r="I5" s="78"/>
     </row>
-    <row r="6" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E6" s="117" t="s">
+    <row r="6" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="124" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
+      <c r="F6" s="124"/>
+      <c r="G6" s="124"/>
       <c r="H6" s="73"/>
       <c r="I6" s="78"/>
     </row>
-    <row r="7" spans="1:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="E7" s="79"/>
       <c r="F7" s="80"/>
       <c r="G7" s="81" t="s">
@@ -3782,47 +4389,47 @@
       <c r="H7" s="73"/>
       <c r="I7" s="78"/>
     </row>
-    <row r="8" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E8" s="111" t="s">
+    <row r="8" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="118" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="111"/>
-      <c r="G8" s="111"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
       <c r="H8" s="73"/>
       <c r="I8" s="78"/>
     </row>
-    <row r="9" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E9" s="111" t="s">
+    <row r="9" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="118" t="s">
         <v>44</v>
       </c>
-      <c r="F9" s="111"/>
-      <c r="G9" s="111"/>
+      <c r="F9" s="118"/>
+      <c r="G9" s="118"/>
       <c r="H9" s="73"/>
       <c r="I9" s="78"/>
     </row>
-    <row r="10" spans="1:20" ht="14" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E10" s="111" t="s">
+    <row r="10" spans="1:19" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="118" t="s">
         <v>45</v>
       </c>
-      <c r="F10" s="111"/>
-      <c r="G10" s="111"/>
+      <c r="F10" s="118"/>
+      <c r="G10" s="118"/>
       <c r="H10" s="73"/>
       <c r="I10" s="78"/>
     </row>
-    <row r="11" spans="1:20" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="82"/>
       <c r="B11" s="82"/>
       <c r="C11" s="82"/>
       <c r="D11" s="82"/>
-      <c r="E11" s="112" t="s">
+      <c r="E11" s="119" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="112"/>
-      <c r="G11" s="112"/>
+      <c r="F11" s="119"/>
+      <c r="G11" s="119"/>
       <c r="H11" s="83"/>
       <c r="I11" s="74"/>
     </row>
-    <row r="12" spans="1:20" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:19" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="84"/>
       <c r="B12" s="84"/>
       <c r="C12" s="84"/>
@@ -3832,148 +4439,141 @@
       <c r="G12" s="84"/>
       <c r="H12" s="84"/>
       <c r="I12" s="84"/>
-      <c r="J12" s="85"/>
+      <c r="J12" s="84"/>
       <c r="K12" s="84"/>
       <c r="L12" s="84"/>
-      <c r="M12" s="84"/>
-      <c r="N12" s="86"/>
-      <c r="O12" s="113" t="s">
+      <c r="M12" s="85"/>
+      <c r="N12" s="120" t="s">
         <v>47</v>
       </c>
-      <c r="P12" s="113"/>
-      <c r="Q12" s="113"/>
-      <c r="R12" s="113"/>
-      <c r="S12" s="113"/>
-      <c r="T12" s="113"/>
-    </row>
-    <row r="13" spans="1:20" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="87" t="s">
+      <c r="O12" s="120"/>
+      <c r="P12" s="120"/>
+      <c r="Q12" s="120"/>
+      <c r="R12" s="120"/>
+      <c r="S12" s="120"/>
+    </row>
+    <row r="13" spans="1:19" ht="54.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="86" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="87" t="s">
+      <c r="B13" s="86" t="s">
         <v>49</v>
       </c>
-      <c r="C13" s="87" t="s">
+      <c r="C13" s="86" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="D13" s="86" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="87" t="s">
+      <c r="E13" s="86" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="87" t="s">
+      <c r="F13" s="86" t="s">
         <v>53</v>
       </c>
-      <c r="G13" s="88" t="s">
+      <c r="G13" s="87" t="s">
         <v>54</v>
       </c>
-      <c r="H13" s="87"/>
-      <c r="I13" s="87" t="s">
+      <c r="H13" s="86"/>
+      <c r="I13" s="86" t="s">
         <v>55</v>
       </c>
-      <c r="J13" s="89" t="s">
+      <c r="J13" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="K13" s="87" t="s">
+      <c r="K13" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="L13" s="87" t="s">
+      <c r="L13" s="86" t="s">
         <v>58</v>
       </c>
-      <c r="M13" s="87" t="s">
+      <c r="M13" s="88"/>
+      <c r="N13" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="N13" s="90"/>
-      <c r="O13" s="87" t="s">
+      <c r="O13" s="86" t="s">
         <v>60</v>
       </c>
-      <c r="P13" s="87" t="s">
+      <c r="P13" s="86" t="s">
         <v>61</v>
       </c>
-      <c r="Q13" s="87" t="s">
+      <c r="Q13" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="R13" s="87" t="s">
+      <c r="R13" s="86" t="s">
+        <v>57</v>
+      </c>
+      <c r="S13" s="102" t="s">
         <v>63</v>
       </c>
-      <c r="S13" s="87" t="s">
-        <v>58</v>
-      </c>
-      <c r="T13" s="119" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="120"/>
-      <c r="B14" s="120"/>
-      <c r="C14" s="120"/>
-      <c r="D14" s="120"/>
-      <c r="E14" s="120"/>
-      <c r="F14" s="120"/>
-      <c r="G14" s="120"/>
-      <c r="H14" s="121"/>
-      <c r="I14" s="122"/>
-      <c r="J14" s="123" t="s">
-        <v>65</v>
-      </c>
-      <c r="K14" s="124"/>
-      <c r="L14" s="125"/>
-      <c r="M14" s="126"/>
-      <c r="N14" s="127"/>
-      <c r="O14" s="122"/>
-      <c r="P14" s="128"/>
-      <c r="Q14" s="128"/>
-      <c r="R14" s="124"/>
-      <c r="S14" s="125"/>
-      <c r="T14" s="126"/>
-    </row>
-    <row r="15" spans="1:20" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="N15" s="92"/>
-    </row>
-    <row r="16" spans="1:20" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N16" s="94"/>
-    </row>
-    <row r="17" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N17" s="94"/>
-    </row>
-    <row r="18" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N18" s="94"/>
-    </row>
-    <row r="19" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N19" s="94"/>
-    </row>
-    <row r="20" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N20" s="94"/>
-    </row>
-    <row r="21" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N21" s="94"/>
-    </row>
-    <row r="22" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N22" s="94"/>
-    </row>
-    <row r="23" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N23" s="94"/>
-    </row>
-    <row r="24" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N24" s="94"/>
-    </row>
-    <row r="25" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N25" s="94"/>
-    </row>
-    <row r="26" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N26" s="94"/>
-    </row>
-    <row r="27" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N27" s="94"/>
-    </row>
-    <row r="28" spans="14:14" s="93" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="N28" s="94"/>
-    </row>
-    <row r="29" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="14:14" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    </row>
+    <row r="14" spans="1:19" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="103"/>
+      <c r="B14" s="103"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="103"/>
+      <c r="E14" s="103"/>
+      <c r="F14" s="103"/>
+      <c r="G14" s="103"/>
+      <c r="H14" s="104"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="106"/>
+      <c r="K14" s="107"/>
+      <c r="L14" s="108"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="105"/>
+      <c r="O14" s="110"/>
+      <c r="P14" s="110"/>
+      <c r="Q14" s="106"/>
+      <c r="R14" s="107"/>
+      <c r="S14" s="108"/>
+    </row>
+    <row r="15" spans="1:19" s="89" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="M15" s="90"/>
+    </row>
+    <row r="16" spans="1:19" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M16" s="92"/>
+    </row>
+    <row r="17" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M17" s="92"/>
+    </row>
+    <row r="18" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M18" s="92"/>
+    </row>
+    <row r="19" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M19" s="92"/>
+    </row>
+    <row r="20" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M20" s="92"/>
+    </row>
+    <row r="21" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M21" s="92"/>
+    </row>
+    <row r="22" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M22" s="92"/>
+    </row>
+    <row r="23" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M23" s="92"/>
+    </row>
+    <row r="24" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M24" s="92"/>
+    </row>
+    <row r="25" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M25" s="92"/>
+    </row>
+    <row r="26" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M26" s="92"/>
+    </row>
+    <row r="27" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M27" s="92"/>
+    </row>
+    <row r="28" spans="13:13" s="91" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="M28" s="92"/>
+    </row>
+    <row r="29" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="13:13" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4054,16 +4654,13 @@
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="E10:G10"/>
     <mergeCell ref="E11:G11"/>
-    <mergeCell ref="O12:T12"/>
+    <mergeCell ref="N12:S12"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="E3:G3"/>
     <mergeCell ref="E5:G5"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="E8:G8"/>
   </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="J13" location="'QA Tags'!A1" display="Tag for Findings " xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <drawing r:id="rId1"/>
@@ -4271,7 +4868,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1001" r:id="rId12" name="Check Box -23">
+            <control shapeId="2066" r:id="rId12" name="Check Box 18">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 27">
                 <anchor moveWithCells="1">
                   <from>
@@ -4293,7 +4890,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1002" r:id="rId13" name="Check Box -22">
+            <control shapeId="2065" r:id="rId13" name="Check Box 17">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 29">
                 <anchor moveWithCells="1">
                   <from>
@@ -4315,7 +4912,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1003" r:id="rId14" name="Check Box -21">
+            <control shapeId="2064" r:id="rId14" name="Check Box 16">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 39">
                 <anchor moveWithCells="1">
                   <from>
@@ -4337,7 +4934,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1004" r:id="rId15" name="Check Box -20">
+            <control shapeId="2063" r:id="rId15" name="Check Box 15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 44">
                 <anchor moveWithCells="1">
                   <from>
@@ -4359,7 +4956,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1005" r:id="rId16" name="Check Box -19">
+            <control shapeId="2062" r:id="rId16" name="Check Box 14">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 1">
                 <anchor moveWithCells="1">
                   <from>
@@ -4381,7 +4978,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1006" r:id="rId17" name="Check Box -18">
+            <control shapeId="2061" r:id="rId17" name="Check Box 13">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 2">
                 <anchor moveWithCells="1">
                   <from>
@@ -4403,7 +5000,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1007" r:id="rId18" name="Check Box -17">
+            <control shapeId="2060" r:id="rId18" name="Check Box 12">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 21">
                 <anchor moveWithCells="1">
                   <from>
@@ -4425,7 +5022,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1008" r:id="rId19" name="Check Box -16">
+            <control shapeId="2059" r:id="rId19" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 62">
                 <anchor moveWithCells="1">
                   <from>
@@ -4447,7 +5044,205 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1009" r:id="rId20" name="Check Box -15">
+            <control shapeId="2058" r:id="rId20" name="Check Box 10">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 64">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1001" r:id="rId21" name="Check Box -23">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 27">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1002" r:id="rId22" name="Check Box -22">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 29">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1003" r:id="rId23" name="Check Box -21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 39">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1004" r:id="rId24" name="Check Box -20">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 44">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1005" r:id="rId25" name="Check Box -19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 1">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1006" r:id="rId26" name="Check Box -18">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 2">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1007" r:id="rId27" name="Check Box -17">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 21">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1008" r:id="rId28" name="Check Box -16">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 62">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1009" r:id="rId29" name="Check Box -15">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 64">
                 <anchor moveWithCells="1">
                   <from>
@@ -4477,7 +5272,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
@@ -4489,63 +5284,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="123" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="118" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="118"/>
+      <c r="A1" s="125" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="125"/>
       <c r="C1" s="17"/>
       <c r="D1" s="17"/>
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="95" t="s">
+      <c r="A2" s="93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="94" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A3" s="95" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="96" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="96" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A3" s="97" t="s">
+    </row>
+    <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A4" s="97" t="s">
         <v>68</v>
       </c>
-      <c r="B3" s="98" t="s">
+      <c r="B4" s="98" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A4" s="99" t="s">
+    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" s="99" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="100" t="s">
+      <c r="B5" s="98" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A5" s="101" t="s">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.2">
+      <c r="A6" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="100" t="s">
+      <c r="B6" s="98" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.2">
-      <c r="A6" s="99" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="100" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="100" t="s">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="101" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="102" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="103" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated with qa branch version
</commit_message>
<xml_diff>
--- a/inst/extdata/QA_Template_Coded_Analysis.xlsx
+++ b/inst/extdata/QA_Template_Coded_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jzadra41/Documents/R Projects/integral-private/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9572DE83-A1BF-E24E-B4C7-5A05A9ACFAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2EF8362-4AC9-CE42-9AA9-29D5A0A5CA2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="18860" yWindow="500" windowWidth="38780" windowHeight="22540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1513,7 +1513,43 @@
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
+<file path=xl/ctrlProps/ctrlProp28.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp29.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
 <file path=xl/ctrlProps/ctrlProp3.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp30.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp31.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" lockText="1" noThreeD="1"/>
 </file>
 
@@ -3490,6 +3526,609 @@
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
                   <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00000A080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2075" name="Check Box 27" descr="Check Box 27" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2075"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001B080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2074" name="Check Box 26" descr="Check Box 29" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2074"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00001A080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2073" name="Check Box 25" descr="Check Box 39" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2073"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000019080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2072" name="Check Box 24" descr="Check Box 44" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2072"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000018080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2071" name="Check Box 23" descr="Check Box 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2071"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000017080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2070" name="Check Box 22" descr="Check Box 2" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2070"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000016080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2069" name="Check Box 21" descr="Check Box 21" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2069"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000015080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2068" name="Check Box 20" descr="Check Box 62" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2068"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000014080000}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>0</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2067" name="Check Box 19" descr="Check Box 64" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s2067"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000013080000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -5066,7 +5705,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1001" r:id="rId21" name="Check Box -23">
+            <control shapeId="2075" r:id="rId21" name="Check Box 27">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 27">
                 <anchor moveWithCells="1">
                   <from>
@@ -5088,7 +5727,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1002" r:id="rId22" name="Check Box -22">
+            <control shapeId="2074" r:id="rId22" name="Check Box 26">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 29">
                 <anchor moveWithCells="1">
                   <from>
@@ -5110,7 +5749,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1003" r:id="rId23" name="Check Box -21">
+            <control shapeId="2073" r:id="rId23" name="Check Box 25">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 39">
                 <anchor moveWithCells="1">
                   <from>
@@ -5132,7 +5771,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1004" r:id="rId24" name="Check Box -20">
+            <control shapeId="2072" r:id="rId24" name="Check Box 24">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 44">
                 <anchor moveWithCells="1">
                   <from>
@@ -5154,7 +5793,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1005" r:id="rId25" name="Check Box -19">
+            <control shapeId="2071" r:id="rId25" name="Check Box 23">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 1">
                 <anchor moveWithCells="1">
                   <from>
@@ -5176,7 +5815,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1006" r:id="rId26" name="Check Box -18">
+            <control shapeId="2070" r:id="rId26" name="Check Box 22">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 2">
                 <anchor moveWithCells="1">
                   <from>
@@ -5198,7 +5837,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1007" r:id="rId27" name="Check Box -17">
+            <control shapeId="2069" r:id="rId27" name="Check Box 21">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 21">
                 <anchor moveWithCells="1">
                   <from>
@@ -5220,7 +5859,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1008" r:id="rId28" name="Check Box -16">
+            <control shapeId="2068" r:id="rId28" name="Check Box 20">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 62">
                 <anchor moveWithCells="1">
                   <from>
@@ -5242,7 +5881,205 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1009" r:id="rId29" name="Check Box -15">
+            <control shapeId="2067" r:id="rId29" name="Check Box 19">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 64">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1001" r:id="rId30" name="Check Box 27">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 27">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1002" r:id="rId31" name="Check Box 29">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 29">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1003" r:id="rId32" name="Check Box 39">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 39">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1004" r:id="rId33" name="Check Box 44">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 44">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1005" r:id="rId34" name="Check Box 1">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 1">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1006" r:id="rId35" name="Check Box 2">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 2">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1007" r:id="rId36" name="Check Box 21">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 21">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1008" r:id="rId37" name="Check Box 62">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 62">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>0</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1009" r:id="rId38" name="Check Box 64">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0" altText="Check Box 64">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>